<commit_message>
mean anomaly saturn moons
</commit_message>
<xml_diff>
--- a/src/app/scene/data/saturn.xlsx
+++ b/src/app/scene/data/saturn.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="434">
   <si>
     <t>Order</t>
   </si>
@@ -1275,6 +1275,57 @@
   </si>
   <si>
     <t>275.5</t>
+  </si>
+  <si>
+    <t>341.3</t>
+  </si>
+  <si>
+    <t>92.56</t>
+  </si>
+  <si>
+    <t>132.4</t>
+  </si>
+  <si>
+    <t>301.6</t>
+  </si>
+  <si>
+    <t>118.0</t>
+  </si>
+  <si>
+    <t>298.6</t>
+  </si>
+  <si>
+    <t>357.2</t>
+  </si>
+  <si>
+    <t>231.7</t>
+  </si>
+  <si>
+    <t>26.40</t>
+  </si>
+  <si>
+    <t>134.5</t>
+  </si>
+  <si>
+    <t>84.64</t>
+  </si>
+  <si>
+    <t>162.7</t>
+  </si>
+  <si>
+    <t>136.2</t>
+  </si>
+  <si>
+    <t>114.7</t>
+  </si>
+  <si>
+    <t>32.50</t>
+  </si>
+  <si>
+    <t>314.4</t>
+  </si>
+  <si>
+    <t>306.6</t>
   </si>
 </sst>
 </file>
@@ -1557,24 +1608,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1597,6 +1630,24 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1880,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1941,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="35" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -1902,7 +1953,7 @@
       <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="38" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1910,7 +1961,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1920,17 +1971,17 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="31"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="29"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="32"/>
+      <c r="F3" s="40"/>
       <c r="G3" t="s">
         <v>413</v>
       </c>
@@ -1969,7 +2020,7 @@
       <c r="F4" s="7">
         <v>0</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="34">
         <v>0</v>
       </c>
       <c r="H4" t="str">
@@ -1977,8 +2028,8 @@
         <v>S_2009_S_1</v>
       </c>
       <c r="I4" t="str">
-        <f>LOWER(SUBSTITUTE(SUBSTITUTE(B4," ","-"),"/","/"))</f>
-        <v>s/2009-s-1</v>
+        <f>LOWER(SUBSTITUTE(SUBSTITUTE(B4," ","-"),"/","_"))</f>
+        <v>s_2009-s-1</v>
       </c>
       <c r="J4" s="26" t="str">
         <f>SUBSTITUTE(C4/2,",",".")</f>
@@ -2001,14 +2052,14 @@
   semiMajorAxis: "&amp;E4&amp;",
   eccentricity: "&amp;F4&amp;",
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: "&amp;G4&amp;",
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
 };
 "</f>
         <v xml:space="preserve">export const S_2009_S_1: CelestialBody = {
-  id: 's/2009-s-1',
+  id: 's_2009-s-1',
   position: {
     x: 0,
     y: 0
@@ -2019,7 +2070,7 @@
   semiMajorAxis: 117000,
   eccentricity: 0,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 0,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2047,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" ref="G5:G68" si="0">IFERROR(VLOOKUP(B5,$B$89:$F$151,5,FALSE),"null")</f>
+        <f t="shared" ref="G5:G63" si="0">IFERROR(VLOOKUP(B5,$B$89:$F$151,5,FALSE),"null")</f>
         <v>351.187</v>
       </c>
       <c r="H5" t="str">
@@ -2055,7 +2106,7 @@
         <v>PAN</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" ref="I5:I63" si="2">LOWER(SUBSTITUTE(SUBSTITUTE(B5," ","-"),"/","/"))</f>
+        <f t="shared" ref="I5:I68" si="2">LOWER(SUBSTITUTE(SUBSTITUTE(B5," ","-"),"/","_"))</f>
         <v>pan</v>
       </c>
       <c r="J5" s="26" t="str">
@@ -2067,7 +2118,7 @@
         <v>4.95e15</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" ref="L5:L63" si="5">"export const " &amp; H5 &amp; ": CelestialBody = {
+        <f t="shared" ref="L5:L68" si="5">"export const " &amp; H5 &amp; ": CelestialBody = {
   id: '" &amp; I5 &amp; "',
   position: {
     x: 0,
@@ -2079,7 +2130,7 @@
   semiMajorAxis: "&amp;E5&amp;",
   eccentricity: "&amp;F5&amp;",
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: "&amp;G5&amp;",
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2097,7 +2148,7 @@
   semiMajorAxis: 133584,
   eccentricity: 0,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 351.187,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2158,7 +2209,7 @@
   semiMajorAxis: 136505,
   eccentricity: 0,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 113.790,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2219,7 +2270,7 @@
   semiMajorAxis: 137670,
   eccentricity: 0.0012,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 283.282,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2280,7 +2331,7 @@
   semiMajorAxis: 139380,
   eccentricity: 0.0022,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 96.886,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2341,7 +2392,7 @@
   semiMajorAxis: 141720,
   eccentricity: 0.0042,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 125.112,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2402,7 +2453,7 @@
   semiMajorAxis: 151422,
   eccentricity: 0.0098,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 80.377,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2463,7 +2514,7 @@
   semiMajorAxis: 151472,
   eccentricity: 0.0068,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 17.342,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2524,7 +2575,7 @@
   semiMajorAxis: 167500,
   eccentricity: 0.0004,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 322.771,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2585,7 +2636,7 @@
   semiMajorAxis: 185404,
   eccentricity: 0.0202,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 14.848,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2646,7 +2697,7 @@
   semiMajorAxis: 194440,
   eccentricity: 0.0001,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 71.189,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2707,7 +2758,7 @@
   semiMajorAxis: 197700,
   eccentricity: 0.0011,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 190.473,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2768,7 +2819,7 @@
   semiMajorAxis: 212280,
   eccentricity: 0.004,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 356.229,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2829,7 +2880,7 @@
   semiMajorAxis: 237950,
   eccentricity: 0.0047,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 199.686,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2890,7 +2941,7 @@
   semiMajorAxis: 294619,
   eccentricity: 0.0001,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 243.367,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2951,7 +3002,7 @@
   semiMajorAxis: 294619,
   eccentricity: 0,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 260.157,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3012,7 +3063,7 @@
   semiMajorAxis: 294619,
   eccentricity: 0,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 156.660,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3073,7 +3124,7 @@
   semiMajorAxis: 377396,
   eccentricity: 0.0022,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 322.232,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3134,7 +3185,7 @@
   semiMajorAxis: 377396,
   eccentricity: 0.0022,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 43.186,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3195,7 +3246,7 @@
   semiMajorAxis: 377396,
   eccentricity: 0.0192,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 89.307,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3256,7 +3307,7 @@
   semiMajorAxis: 527108,
   eccentricity: 0.0013,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 179.781,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3317,7 +3368,7 @@
   semiMajorAxis: 1221930,
   eccentricity: 0.0288,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 163.310,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3378,7 +3429,7 @@
   semiMajorAxis: 1481010,
   eccentricity: 0.123,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 86.342,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3439,7 +3490,7 @@
   semiMajorAxis: 3560820,
   eccentricity: 0.0286,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 201.789,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3500,7 +3551,7 @@
   semiMajorAxis: 11307500,
   eccentricity: 0.1521,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 172.018,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3561,7 +3612,7 @@
   semiMajorAxis: 11348500,
   eccentricity: 0.3758,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 17.328,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3622,7 +3673,7 @@
   semiMajorAxis: 12905900,
   eccentricity: 0.1604,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 53.038,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3683,7 +3734,7 @@
   semiMajorAxis: 15012800,
   eccentricity: 0.4826,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 321.654,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3744,7 +3795,7 @@
   semiMajorAxis: 15563600,
   eccentricity: 0.2755,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 114.689,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3771,7 +3822,7 @@
       <c r="F33" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G33" s="40" t="s">
+      <c r="G33" s="34" t="s">
         <v>414</v>
       </c>
       <c r="H33" t="str">
@@ -3780,7 +3831,7 @@
       </c>
       <c r="I33" t="str">
         <f t="shared" si="2"/>
-        <v>s/2004-s-37</v>
+        <v>s_2004-s-37</v>
       </c>
       <c r="J33" s="26" t="str">
         <f t="shared" si="3"/>
@@ -3793,7 +3844,7 @@
       <c r="L33" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_37: CelestialBody = {
-  id: 's/2004-s-37',
+  id: 's_2004-s-37',
   position: {
     x: 0,
     y: 0
@@ -3804,7 +3855,7 @@
   semiMajorAxis: 15822400,
   eccentricity: 0.5265,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 326.7,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3841,7 +3892,7 @@
       </c>
       <c r="I34" t="str">
         <f t="shared" si="2"/>
-        <v>s/2007-s-2</v>
+        <v>s_2007-s-2</v>
       </c>
       <c r="J34" s="26" t="str">
         <f t="shared" si="3"/>
@@ -3854,7 +3905,7 @@
       <c r="L34" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2007_S_2: CelestialBody = {
-  id: 's/2007-s-2',
+  id: 's_2007-s-2',
   position: {
     x: 0,
     y: 0
@@ -3865,7 +3916,7 @@
   semiMajorAxis: 15971500,
   eccentricity: 0.2465,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 84.066,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3926,7 +3977,7 @@
   semiMajorAxis: 16222700,
   eccentricity: 0.5807,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 32.828,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -3987,7 +4038,7 @@
   semiMajorAxis: 16900900,
   eccentricity: 0.3813,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 168.045,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4014,7 +4065,7 @@
       <c r="F37" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G37" s="40" t="s">
+      <c r="G37" s="34" t="s">
         <v>415</v>
       </c>
       <c r="H37" t="str">
@@ -4023,7 +4074,7 @@
       </c>
       <c r="I37" t="str">
         <f t="shared" si="2"/>
-        <v>s/2004-s-29</v>
+        <v>s_2004-s-29</v>
       </c>
       <c r="J37" s="26" t="str">
         <f t="shared" si="3"/>
@@ -4036,7 +4087,7 @@
       <c r="L37" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_29: CelestialBody = {
-  id: 's/2004-s-29',
+  id: 's_2004-s-29',
   position: {
     x: 0,
     y: 0
@@ -4047,7 +4098,7 @@
   semiMajorAxis: 17202800,
   eccentricity: 0.4269,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 211.6,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4108,7 +4159,7 @@
   semiMajorAxis: 17438300,
   eccentricity: 0.4402,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 44.965,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4135,7 +4186,7 @@
       <c r="F39" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="G39" s="40" t="s">
+      <c r="G39" s="34" t="s">
         <v>416</v>
       </c>
       <c r="H39" t="str">
@@ -4144,7 +4195,7 @@
       </c>
       <c r="I39" t="str">
         <f t="shared" si="2"/>
-        <v>s/2004-s-31</v>
+        <v>s_2004-s-31</v>
       </c>
       <c r="J39" s="26" t="str">
         <f t="shared" si="3"/>
@@ -4157,7 +4208,7 @@
       <c r="L39" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_31: CelestialBody = {
-  id: 's/2004-s-31',
+  id: 's_2004-s-31',
   position: {
     x: 0,
     y: 0
@@ -4168,7 +4219,7 @@
   semiMajorAxis: 17449700,
   eccentricity: 0.2525,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 275.5,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4229,7 +4280,7 @@
   semiMajorAxis: 17705500,
   eccentricity: 0.452,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 294.829,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4290,7 +4341,7 @@
   semiMajorAxis: 17724200,
   eccentricity: 0.1373,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 161.020,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4351,7 +4402,7 @@
   semiMajorAxis: 17937000,
   eccentricity: 0.5293,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 201.288,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4412,7 +4463,7 @@
   semiMajorAxis: 18243800,
   eccentricity: 0.4799,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 265.783,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4473,7 +4524,7 @@
   semiMajorAxis: 18348800,
   eccentricity: 0.3582,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 291.841,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4534,7 +4585,7 @@
   semiMajorAxis: 18379000,
   eccentricity: 0.3331,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 314.541,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4595,7 +4646,7 @@
   semiMajorAxis: 18470800,
   eccentricity: 0.1787,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 92.821,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4632,7 +4683,7 @@
       </c>
       <c r="I47" t="str">
         <f t="shared" si="2"/>
-        <v>s/2004-s-13</v>
+        <v>s_2004-s-13</v>
       </c>
       <c r="J47" s="26" t="str">
         <f t="shared" si="3"/>
@@ -4645,7 +4696,7 @@
       <c r="L47" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_13: CelestialBody = {
-  id: 's/2004-s-13',
+  id: 's_2004-s-13',
   position: {
     x: 0,
     y: 0
@@ -4656,7 +4707,7 @@
   semiMajorAxis: 18594700,
   eccentricity: 0.29,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 41.077,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4693,7 +4744,7 @@
       </c>
       <c r="I48" t="str">
         <f t="shared" si="2"/>
-        <v>s/2006-s-1</v>
+        <v>s_2006-s-1</v>
       </c>
       <c r="J48" s="26" t="str">
         <f t="shared" si="3"/>
@@ -4706,7 +4757,7 @@
       <c r="L48" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2006_S_1: CelestialBody = {
-  id: 's/2006-s-1',
+  id: 's_2006-s-1',
   position: {
     x: 0,
     y: 0
@@ -4717,7 +4768,7 @@
   semiMajorAxis: 18839700,
   eccentricity: 0.0972,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 96.596,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4754,7 +4805,7 @@
       </c>
       <c r="I49" t="str">
         <f t="shared" si="2"/>
-        <v>s/2007-s-3</v>
+        <v>s_2007-s-3</v>
       </c>
       <c r="J49" s="26" t="str">
         <f t="shared" si="3"/>
@@ -4767,7 +4818,7 @@
       <c r="L49" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2007_S_3: CelestialBody = {
-  id: 's/2007-s-3',
+  id: 's_2007-s-3',
   position: {
     x: 0,
     y: 0
@@ -4778,7 +4829,7 @@
   semiMajorAxis: 19143500,
   eccentricity: 0.1671,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 292.691,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4839,7 +4890,7 @@
   semiMajorAxis: 19166800,
   eccentricity: 0.1445,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 321.133,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4866,14 +4917,16 @@
       <c r="F51" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G51" s="40"/>
+      <c r="G51" s="34" t="s">
+        <v>417</v>
+      </c>
       <c r="H51" t="str">
         <f t="shared" si="1"/>
         <v>S_2004_S_20</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="2"/>
-        <v>s/2004-s-20</v>
+        <v>s_2004-s-20</v>
       </c>
       <c r="J51" s="26" t="str">
         <f t="shared" si="3"/>
@@ -4886,7 +4939,7 @@
       <c r="L51" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_20: CelestialBody = {
-  id: 's/2004-s-20',
+  id: 's_2004-s-20',
   position: {
     x: 0,
     y: 0
@@ -4897,7 +4950,7 @@
   semiMajorAxis: 19188100,
   eccentricity: 0.1976,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 341.3,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -4958,7 +5011,7 @@
   semiMajorAxis: 19197900,
   eccentricity: 0.2148,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 198.750,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5019,7 +5072,7 @@
   semiMajorAxis: 19226600,
   eccentricity: 0.299,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 114.172,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5080,7 +5133,7 @@
   semiMajorAxis: 19290200,
   eccentricity: 0.1399,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 306.494,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5141,7 +5194,7 @@
   semiMajorAxis: 19435300,
   eccentricity: 0.3295,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 163.640,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5178,7 +5231,7 @@
       </c>
       <c r="I56" t="str">
         <f t="shared" si="2"/>
-        <v>s/2004-s-17</v>
+        <v>s_2004-s-17</v>
       </c>
       <c r="J56" s="26" t="str">
         <f t="shared" si="3"/>
@@ -5191,7 +5244,7 @@
       <c r="L56" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_17: CelestialBody = {
-  id: 's/2004-s-17',
+  id: 's_2004-s-17',
   position: {
     x: 0,
     y: 0
@@ -5202,7 +5255,7 @@
   semiMajorAxis: 19574300,
   eccentricity: 0.1916,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 228.545,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5239,7 +5292,7 @@
       </c>
       <c r="I57" t="str">
         <f t="shared" si="2"/>
-        <v>s/2004-s-12</v>
+        <v>s_2004-s-12</v>
       </c>
       <c r="J57" s="26" t="str">
         <f t="shared" si="3"/>
@@ -5252,7 +5305,7 @@
       <c r="L57" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_12: CelestialBody = {
-  id: 's/2004-s-12',
+  id: 's_2004-s-12',
   position: {
     x: 0,
     y: 0
@@ -5263,7 +5316,7 @@
   semiMajorAxis: 19736400,
   eccentricity: 0.3929,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 1.599,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5290,14 +5343,16 @@
       <c r="F58" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="G58" s="40"/>
+      <c r="G58" s="34" t="s">
+        <v>418</v>
+      </c>
       <c r="H58" t="str">
         <f t="shared" si="1"/>
         <v>S_2004_S_27</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" si="2"/>
-        <v>s/2004-s-27</v>
+        <v>s_2004-s-27</v>
       </c>
       <c r="J58" s="26" t="str">
         <f t="shared" si="3"/>
@@ -5310,7 +5365,7 @@
       <c r="L58" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_27: CelestialBody = {
-  id: 's/2004-s-27',
+  id: 's_2004-s-27',
   position: {
     x: 0,
     y: 0
@@ -5321,7 +5376,7 @@
   semiMajorAxis: 19982800,
   eccentricity: 0.1364,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 92.56,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5382,7 +5437,7 @@
   semiMajorAxis: 20101600,
   eccentricity: 0.1756,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 282.813,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5443,7 +5498,7 @@
   semiMajorAxis: 20236700,
   eccentricity: 0.4332,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 30.075,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5504,7 +5559,7 @@
   semiMajorAxis: 20432100,
   eccentricity: 0.7072,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 239.156,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5541,7 +5596,7 @@
       </c>
       <c r="I62" t="str">
         <f t="shared" si="2"/>
-        <v>s/2004-s-7</v>
+        <v>s_2004-s-7</v>
       </c>
       <c r="J62" s="26" t="str">
         <f t="shared" si="3"/>
@@ -5554,7 +5609,7 @@
       <c r="L62" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_7: CelestialBody = {
-  id: 's/2004-s-7',
+  id: 's_2004-s-7',
   position: {
     x: 0,
     y: 0
@@ -5565,7 +5620,7 @@
   semiMajorAxis: 20576700,
   eccentricity: 0.4998,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 79.762,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5626,7 +5681,7 @@
   semiMajorAxis: 20598900,
   eccentricity: 0.2379,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 26.017,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5653,44 +5708,29 @@
       <c r="F64" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="G64" s="40"/>
+      <c r="G64" s="34" t="s">
+        <v>419</v>
+      </c>
       <c r="H64" t="str">
         <f t="shared" ref="H64:H85" si="6">UPPER(SUBSTITUTE(SUBSTITUTE(B64," ","_"),"/","_"))</f>
         <v>S_2004_S_30</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" ref="I64:I85" si="7">LOWER(SUBSTITUTE(SUBSTITUTE(B64," ","-"),"/","/"))</f>
-        <v>s/2004-s-30</v>
+        <f t="shared" si="2"/>
+        <v>s_2004-s-30</v>
       </c>
       <c r="J64" s="26" t="str">
-        <f t="shared" ref="J64:J85" si="8">SUBSTITUTE(C64/2,",",".")</f>
+        <f t="shared" ref="J64:J85" si="7">SUBSTITUTE(C64/2,",",".")</f>
         <v>1.5</v>
       </c>
       <c r="K64" t="str">
-        <f t="shared" ref="K64:K85" si="9">SUBSTITUTE(CONCATENATE(D64,"e15"),",",".")</f>
+        <f t="shared" ref="K64:K85" si="8">SUBSTITUTE(CONCATENATE(D64,"e15"),",",".")</f>
         <v>0.03e15</v>
       </c>
       <c r="L64" t="str">
-        <f t="shared" ref="L64:L85" si="10">"export const " &amp; H64 &amp; ": CelestialBody = {
-  id: '" &amp; I64 &amp; "',
-  position: {
-    x: 0,
-    y: 0" &amp; "
-  },
-  speed: 0, // TODO
-  mass: "&amp;K64&amp;",
-  radius: "&amp;J64&amp;",
-  semiMajorAxis: "&amp;E64&amp;",
-  eccentricity: "&amp;F64&amp;",
-  trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
-  type: CELESTIAL_BODY_TYPE.SATELLITE,
-  satellites: [],
-  orbitBody: null
-};
-"</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_30: CelestialBody = {
-  id: 's/2004-s-30',
+  id: 's_2004-s-30',
   position: {
     x: 0,
     y: 0
@@ -5701,7 +5741,7 @@
   semiMajorAxis: 20733300,
   eccentricity: 0.0859,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 132.4,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5728,27 +5768,29 @@
       <c r="F65" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="G65" s="40"/>
+      <c r="G65" s="34" t="s">
+        <v>421</v>
+      </c>
       <c r="H65" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_22</v>
       </c>
       <c r="I65" t="str">
+        <f t="shared" si="2"/>
+        <v>s_2004-s-22</v>
+      </c>
+      <c r="J65" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-22</v>
-      </c>
-      <c r="J65" s="26" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="K65" t="str">
         <f t="shared" si="8"/>
-        <v>1.5</v>
-      </c>
-      <c r="K65" t="str">
-        <f t="shared" si="9"/>
         <v>0.03e15</v>
       </c>
       <c r="L65" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_22: CelestialBody = {
-  id: 's/2004-s-22',
+  id: 's_2004-s-22',
   position: {
     x: 0,
     y: 0
@@ -5759,7 +5801,7 @@
   semiMajorAxis: 20737100,
   eccentricity: 0.2369,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 118.0,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5786,27 +5828,29 @@
       <c r="F66" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="G66" s="40"/>
+      <c r="G66" s="34" t="s">
+        <v>420</v>
+      </c>
       <c r="H66" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_25</v>
       </c>
       <c r="I66" t="str">
+        <f t="shared" si="2"/>
+        <v>s_2004-s-25</v>
+      </c>
+      <c r="J66" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-25</v>
-      </c>
-      <c r="J66" s="26" t="str">
+        <v>2</v>
+      </c>
+      <c r="K66" t="str">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K66" t="str">
-        <f t="shared" si="9"/>
         <v>0.05e15</v>
       </c>
       <c r="L66" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_25: CelestialBody = {
-  id: 's/2004-s-25',
+  id: 's_2004-s-25',
   position: {
     x: 0,
     y: 0
@@ -5817,7 +5861,7 @@
   semiMajorAxis: 20814800,
   eccentricity: 0.4362,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 301.6,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5844,27 +5888,29 @@
       <c r="F67" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="G67" s="40"/>
+      <c r="G67" s="34" t="s">
+        <v>422</v>
+      </c>
       <c r="H67" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_32</v>
       </c>
       <c r="I67" t="str">
+        <f t="shared" si="2"/>
+        <v>s_2004-s-32</v>
+      </c>
+      <c r="J67" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-32</v>
-      </c>
-      <c r="J67" s="26" t="str">
+        <v>2</v>
+      </c>
+      <c r="K67" t="str">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K67" t="str">
-        <f t="shared" si="9"/>
         <v>0.05e15</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_32: CelestialBody = {
-  id: 's/2004-s-32',
+  id: 's_2004-s-32',
   position: {
     x: 0,
     y: 0
@@ -5875,7 +5921,7 @@
   semiMajorAxis: 20963400,
   eccentricity: 0.2594,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 298.6,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5902,27 +5948,29 @@
       <c r="F68" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="G68" s="40"/>
+      <c r="G68" s="34" t="s">
+        <v>423</v>
+      </c>
       <c r="H68" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_23</v>
       </c>
       <c r="I68" t="str">
+        <f t="shared" si="2"/>
+        <v>s_2004-s-23</v>
+      </c>
+      <c r="J68" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-23</v>
-      </c>
-      <c r="J68" s="26" t="str">
+        <v>2</v>
+      </c>
+      <c r="K68" t="str">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K68" t="str">
-        <f t="shared" si="9"/>
         <v>0.05e15</v>
       </c>
       <c r="L68" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">export const S_2004_S_23: CelestialBody = {
-  id: 's/2004-s-23',
+  id: 's_2004-s-23',
   position: {
     x: 0,
     y: 0
@@ -5933,7 +5981,7 @@
   semiMajorAxis: 21444300,
   eccentricity: 0.4133,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 357.2,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -5961,7 +6009,7 @@
         <v>86</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" ref="G69:G85" si="11">IFERROR(VLOOKUP(B69,$B$89:$F$151,5,FALSE),"null")</f>
+        <f t="shared" ref="G69:G83" si="9">IFERROR(VLOOKUP(B69,$B$89:$F$151,5,FALSE),"null")</f>
         <v>167.147</v>
       </c>
       <c r="H69" t="str">
@@ -5969,21 +6017,38 @@
         <v>S_2006_S_3</v>
       </c>
       <c r="I69" t="str">
+        <f t="shared" ref="I69:I85" si="10">LOWER(SUBSTITUTE(SUBSTITUTE(B69," ","-"),"/","_"))</f>
+        <v>s_2006-s-3</v>
+      </c>
+      <c r="J69" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2006-s-3</v>
-      </c>
-      <c r="J69" s="26" t="str">
+        <v>3</v>
+      </c>
+      <c r="K69" t="str">
         <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="K69" t="str">
-        <f t="shared" si="9"/>
         <v>0.15e15</v>
       </c>
       <c r="L69" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="L69:L85" si="11">"export const " &amp; H69 &amp; ": CelestialBody = {
+  id: '" &amp; I69 &amp; "',
+  position: {
+    x: 0,
+    y: 0" &amp; "
+  },
+  speed: 0, // TODO
+  mass: "&amp;K69&amp;",
+  radius: "&amp;J69&amp;",
+  semiMajorAxis: "&amp;E69&amp;",
+  eccentricity: "&amp;F69&amp;",
+  trueAnomaly: 0,
+  meanAnomaly: "&amp;G69&amp;",
+  type: CELESTIAL_BODY_TYPE.SATELLITE,
+  satellites: [],
+  orbitBody: null
+};
+"</f>
         <v xml:space="preserve">export const S_2006_S_3: CelestialBody = {
-  id: 's/2006-s-3',
+  id: 's_2006-s-3',
   position: {
     x: 0,
     y: 0
@@ -5994,7 +6059,7 @@
   semiMajorAxis: 21607300,
   eccentricity: 0.4533,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 167.147,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6021,27 +6086,29 @@
       <c r="F70" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="G70" s="40"/>
+      <c r="G70" s="34" t="s">
+        <v>424</v>
+      </c>
       <c r="H70" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_35</v>
       </c>
       <c r="I70" t="str">
+        <f t="shared" si="10"/>
+        <v>s_2004-s-35</v>
+      </c>
+      <c r="J70" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-35</v>
-      </c>
-      <c r="J70" s="26" t="str">
+        <v>3</v>
+      </c>
+      <c r="K70" t="str">
         <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="K70" t="str">
-        <f t="shared" si="9"/>
         <v>0.15e15</v>
       </c>
       <c r="L70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const S_2004_S_35: CelestialBody = {
-  id: 's/2004-s-35',
+  id: 's_2004-s-35',
   position: {
     x: 0,
     y: 0
@@ -6052,7 +6119,7 @@
   semiMajorAxis: 21864500,
   eccentricity: 0.203,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 231.7,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6080,7 +6147,7 @@
         <v>87</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>286.021</v>
       </c>
       <c r="H71" t="str">
@@ -6088,19 +6155,19 @@
         <v>KARI</v>
       </c>
       <c r="I71" t="str">
+        <f t="shared" si="10"/>
+        <v>kari</v>
+      </c>
+      <c r="J71" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>kari</v>
-      </c>
-      <c r="J71" s="26" t="str">
+        <v>3</v>
+      </c>
+      <c r="K71" t="str">
         <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="K71" t="str">
-        <f t="shared" si="9"/>
         <v>0.23e15</v>
       </c>
       <c r="L71" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const KARI: CelestialBody = {
   id: 'kari',
   position: {
@@ -6113,7 +6180,7 @@
   semiMajorAxis: 21988000,
   eccentricity: 0.3745,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 286.021,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6140,27 +6207,29 @@
       <c r="F72" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="G72" s="40"/>
+      <c r="G72" s="34" t="s">
+        <v>425</v>
+      </c>
       <c r="H72" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_28</v>
       </c>
       <c r="I72" t="str">
+        <f t="shared" si="10"/>
+        <v>s_2004-s-28</v>
+      </c>
+      <c r="J72" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-28</v>
-      </c>
-      <c r="J72" s="26" t="str">
+        <v>2</v>
+      </c>
+      <c r="K72" t="str">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K72" t="str">
-        <f t="shared" si="9"/>
         <v>0.05e15</v>
       </c>
       <c r="L72" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const S_2004_S_28: CelestialBody = {
-  id: 's/2004-s-28',
+  id: 's_2004-s-28',
   position: {
     x: 0,
     y: 0
@@ -6171,7 +6240,7 @@
   semiMajorAxis: 22134400,
   eccentricity: 0.1249,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 26.40,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6199,7 +6268,7 @@
         <v>89</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>337.237</v>
       </c>
       <c r="H73" t="str">
@@ -6207,19 +6276,19 @@
         <v>LOGE</v>
       </c>
       <c r="I73" t="str">
+        <f t="shared" si="10"/>
+        <v>loge</v>
+      </c>
+      <c r="J73" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>loge</v>
-      </c>
-      <c r="J73" s="26" t="str">
+        <v>2.5</v>
+      </c>
+      <c r="K73" t="str">
         <f t="shared" si="8"/>
-        <v>2.5</v>
-      </c>
-      <c r="K73" t="str">
-        <f t="shared" si="9"/>
         <v>0.15e15</v>
       </c>
       <c r="L73" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const LOGE: CelestialBody = {
   id: 'loge',
   position: {
@@ -6232,7 +6301,7 @@
   semiMajorAxis: 22563800,
   eccentricity: 0.1584,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 337.237,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6259,27 +6328,29 @@
       <c r="F74" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="G74" s="40"/>
+      <c r="G74" s="34" t="s">
+        <v>426</v>
+      </c>
       <c r="H74" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_38</v>
       </c>
       <c r="I74" t="str">
+        <f t="shared" si="10"/>
+        <v>s_2004-s-38</v>
+      </c>
+      <c r="J74" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-38</v>
-      </c>
-      <c r="J74" s="26" t="str">
+        <v>2</v>
+      </c>
+      <c r="K74" t="str">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K74" t="str">
-        <f t="shared" si="9"/>
         <v>0.05e15</v>
       </c>
       <c r="L74" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const S_2004_S_38: CelestialBody = {
-  id: 's/2004-s-38',
+  id: 's_2004-s-38',
   position: {
     x: 0,
     y: 0
@@ -6290,7 +6361,7 @@
   semiMajorAxis: 22616000,
   eccentricity: 0.4084,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 134.5,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6318,7 +6389,7 @@
         <v>91</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>131.678</v>
       </c>
       <c r="H75" t="str">
@@ -6326,19 +6397,19 @@
         <v>FENRIR</v>
       </c>
       <c r="I75" t="str">
+        <f t="shared" si="10"/>
+        <v>fenrir</v>
+      </c>
+      <c r="J75" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>fenrir</v>
-      </c>
-      <c r="J75" s="26" t="str">
+        <v>2</v>
+      </c>
+      <c r="K75" t="str">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K75" t="str">
-        <f t="shared" si="9"/>
         <v>0.05e15</v>
       </c>
       <c r="L75" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const FENRIR: CelestialBody = {
   id: 'fenrir',
   position: {
@@ -6351,7 +6422,7 @@
   semiMajorAxis: 22753400,
   eccentricity: 0.0949,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 131.678,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6379,7 +6450,7 @@
         <v>92</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>228.673</v>
       </c>
       <c r="H76" t="str">
@@ -6387,19 +6458,19 @@
         <v>YMIR</v>
       </c>
       <c r="I76" t="str">
+        <f t="shared" si="10"/>
+        <v>ymir</v>
+      </c>
+      <c r="J76" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>ymir</v>
-      </c>
-      <c r="J76" s="26" t="str">
+        <v>9.5</v>
+      </c>
+      <c r="K76" t="str">
         <f t="shared" si="8"/>
-        <v>9.5</v>
-      </c>
-      <c r="K76" t="str">
-        <f t="shared" si="9"/>
         <v>3.97e15</v>
       </c>
       <c r="L76" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const YMIR: CelestialBody = {
   id: 'ymir',
   position: {
@@ -6412,7 +6483,7 @@
   semiMajorAxis: 22841900,
   eccentricity: 0.3431,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 228.673,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6440,7 +6511,7 @@
         <v>93</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>136.191</v>
       </c>
       <c r="H77" t="str">
@@ -6448,19 +6519,19 @@
         <v>SURTUR</v>
       </c>
       <c r="I77" t="str">
+        <f t="shared" si="10"/>
+        <v>surtur</v>
+      </c>
+      <c r="J77" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>surtur</v>
-      </c>
-      <c r="J77" s="26" t="str">
+        <v>3</v>
+      </c>
+      <c r="K77" t="str">
         <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="K77" t="str">
-        <f t="shared" si="9"/>
         <v>0.15e15</v>
       </c>
       <c r="L77" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const SURTUR: CelestialBody = {
   id: 'surtur',
   position: {
@@ -6473,7 +6544,7 @@
   semiMajorAxis: 23065900,
   eccentricity: 0.3591,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 136.191,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6500,27 +6571,29 @@
       <c r="F78" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="G78" s="40"/>
+      <c r="G78" s="34" t="s">
+        <v>427</v>
+      </c>
       <c r="H78" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_33</v>
       </c>
       <c r="I78" t="str">
+        <f t="shared" si="10"/>
+        <v>s_2004-s-33</v>
+      </c>
+      <c r="J78" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-33</v>
-      </c>
-      <c r="J78" s="26" t="str">
+        <v>2</v>
+      </c>
+      <c r="K78" t="str">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K78" t="str">
-        <f t="shared" si="9"/>
         <v>0.05e15</v>
       </c>
       <c r="L78" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const S_2004_S_33: CelestialBody = {
-  id: 's/2004-s-33',
+  id: 's_2004-s-33',
   position: {
     x: 0,
     y: 0
@@ -6531,7 +6604,7 @@
   semiMajorAxis: 23087600,
   eccentricity: 0.4113,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 84.64,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6558,27 +6631,29 @@
       <c r="F79" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="G79" s="40"/>
+      <c r="G79" s="34" t="s">
+        <v>428</v>
+      </c>
       <c r="H79" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_24</v>
       </c>
       <c r="I79" t="str">
+        <f t="shared" si="10"/>
+        <v>s_2004-s-24</v>
+      </c>
+      <c r="J79" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-24</v>
-      </c>
-      <c r="J79" s="26" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="K79" t="str">
         <f t="shared" si="8"/>
-        <v>1.5</v>
-      </c>
-      <c r="K79" t="str">
-        <f t="shared" si="9"/>
         <v>0.03e15</v>
       </c>
       <c r="L79" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const S_2004_S_24: CelestialBody = {
-  id: 's/2004-s-24',
+  id: 's_2004-s-24',
   position: {
     x: 0,
     y: 0
@@ -6589,7 +6664,7 @@
   semiMajorAxis: 23326300,
   eccentricity: 0.04,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 162.7,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6616,27 +6691,29 @@
       <c r="F80" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="G80" s="40"/>
+      <c r="G80" s="34" t="s">
+        <v>429</v>
+      </c>
       <c r="H80" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_21</v>
       </c>
       <c r="I80" t="str">
+        <f t="shared" si="10"/>
+        <v>s_2004-s-21</v>
+      </c>
+      <c r="J80" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-21</v>
-      </c>
-      <c r="J80" s="26" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="K80" t="str">
         <f t="shared" si="8"/>
-        <v>1.5</v>
-      </c>
-      <c r="K80" t="str">
-        <f t="shared" si="9"/>
         <v>0.03e15</v>
       </c>
       <c r="L80" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const S_2004_S_21: CelestialBody = {
-  id: 's/2004-s-21',
+  id: 's_2004-s-21',
   position: {
     x: 0,
     y: 0
@@ -6647,7 +6724,7 @@
   semiMajorAxis: 23356200,
   eccentricity: 0.3156,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 136.2,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6674,27 +6751,29 @@
       <c r="F81" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="G81" s="40"/>
+      <c r="G81" s="34" t="s">
+        <v>430</v>
+      </c>
       <c r="H81" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_39</v>
       </c>
       <c r="I81" t="str">
+        <f t="shared" si="10"/>
+        <v>s_2004-s-39</v>
+      </c>
+      <c r="J81" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-39</v>
-      </c>
-      <c r="J81" s="26" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="K81" t="str">
         <f t="shared" si="8"/>
-        <v>1.5</v>
-      </c>
-      <c r="K81" t="str">
-        <f t="shared" si="9"/>
         <v>0.03e15</v>
       </c>
       <c r="L81" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const S_2004_S_39: CelestialBody = {
-  id: 's/2004-s-39',
+  id: 's_2004-s-39',
   position: {
     x: 0,
     y: 0
@@ -6705,7 +6784,7 @@
   semiMajorAxis: 23463800,
   eccentricity: 0.0979,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 114.7,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6732,27 +6811,29 @@
       <c r="F82" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="G82" s="40"/>
+      <c r="G82" s="34" t="s">
+        <v>431</v>
+      </c>
       <c r="H82" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_36</v>
       </c>
       <c r="I82" t="str">
+        <f t="shared" si="10"/>
+        <v>s_2004-s-36</v>
+      </c>
+      <c r="J82" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-36</v>
-      </c>
-      <c r="J82" s="26" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="K82" t="str">
         <f t="shared" si="8"/>
-        <v>1.5</v>
-      </c>
-      <c r="K82" t="str">
-        <f t="shared" si="9"/>
         <v>0.03e15</v>
       </c>
       <c r="L82" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const S_2004_S_36: CelestialBody = {
-  id: 's/2004-s-36',
+  id: 's_2004-s-36',
   position: {
     x: 0,
     y: 0
@@ -6763,7 +6844,7 @@
   semiMajorAxis: 23576500,
   eccentricity: 0.7139,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 32.50,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6791,7 +6872,7 @@
         <v>99</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>214.499</v>
       </c>
       <c r="H83" t="str">
@@ -6799,19 +6880,19 @@
         <v>FORNJOT</v>
       </c>
       <c r="I83" t="str">
+        <f t="shared" si="10"/>
+        <v>fornjot</v>
+      </c>
+      <c r="J83" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>fornjot</v>
-      </c>
-      <c r="J83" s="26" t="str">
+        <v>3</v>
+      </c>
+      <c r="K83" t="str">
         <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="K83" t="str">
-        <f t="shared" si="9"/>
         <v>0.15e15</v>
       </c>
       <c r="L83" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const FORNJOT: CelestialBody = {
   id: 'fornjot',
   position: {
@@ -6824,7 +6905,7 @@
   semiMajorAxis: 24451700,
   eccentricity: 0.1613,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 214.499,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6851,27 +6932,29 @@
       <c r="F84" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="G84" s="40"/>
+      <c r="G84" s="34" t="s">
+        <v>432</v>
+      </c>
       <c r="H84" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_34</v>
       </c>
       <c r="I84" t="str">
+        <f t="shared" si="10"/>
+        <v>s_2004-s-34</v>
+      </c>
+      <c r="J84" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-34</v>
-      </c>
-      <c r="J84" s="26" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="K84" t="str">
         <f t="shared" si="8"/>
-        <v>1.5</v>
-      </c>
-      <c r="K84" t="str">
-        <f t="shared" si="9"/>
         <v>0.03e15</v>
       </c>
       <c r="L84" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const S_2004_S_34: CelestialBody = {
-  id: 's/2004-s-34',
+  id: 's_2004-s-34',
   position: {
     x: 0,
     y: 0
@@ -6882,7 +6965,7 @@
   semiMajorAxis: 24865000,
   eccentricity: 0.2015,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 314.4,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6909,27 +6992,29 @@
       <c r="F85" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="G85" s="40"/>
+      <c r="G85" s="34" t="s">
+        <v>433</v>
+      </c>
       <c r="H85" t="str">
         <f t="shared" si="6"/>
         <v>S_2004_S_26</v>
       </c>
       <c r="I85" t="str">
+        <f t="shared" si="10"/>
+        <v>s_2004-s-26</v>
+      </c>
+      <c r="J85" s="26" t="str">
         <f t="shared" si="7"/>
-        <v>s/2004-s-26</v>
-      </c>
-      <c r="J85" s="26" t="str">
+        <v>2</v>
+      </c>
+      <c r="K85" t="str">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K85" t="str">
-        <f t="shared" si="9"/>
         <v>0.05e15</v>
       </c>
       <c r="L85" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">export const S_2004_S_26: CelestialBody = {
-  id: 's/2004-s-26',
+  id: 's_2004-s-26',
   position: {
     x: 0,
     y: 0
@@ -6940,7 +7025,7 @@
   semiMajorAxis: 26701600,
   eccentricity: 0.1726,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 306.6,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -6952,1590 +7037,1590 @@
       <c r="A87" s="25"/>
     </row>
     <row r="89" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B89" s="33" t="s">
+      <c r="B89" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="C89" s="34" t="s">
+      <c r="C89" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="D89" s="34" t="s">
+      <c r="D89" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="E89" s="34" t="s">
+      <c r="E89" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="F89" s="34" t="s">
+      <c r="F89" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="G89" s="34"/>
-      <c r="H89" s="34"/>
-      <c r="I89" s="34"/>
-      <c r="J89" s="34"/>
-      <c r="K89" s="34"/>
-      <c r="L89" s="34"/>
-      <c r="M89" s="34"/>
-      <c r="N89" s="34"/>
-      <c r="O89" s="34"/>
-      <c r="P89" s="35"/>
+      <c r="G89" s="28"/>
+      <c r="H89" s="28"/>
+      <c r="I89" s="28"/>
+      <c r="J89" s="28"/>
+      <c r="K89" s="28"/>
+      <c r="L89" s="28"/>
+      <c r="M89" s="28"/>
+      <c r="N89" s="28"/>
+      <c r="O89" s="28"/>
+      <c r="P89" s="29"/>
     </row>
     <row r="90" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B90" s="33"/>
-      <c r="C90" s="36" t="s">
+      <c r="B90" s="27"/>
+      <c r="C90" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="D90" s="36"/>
-      <c r="E90" s="36" t="s">
+      <c r="D90" s="30"/>
+      <c r="E90" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="F90" s="36" t="s">
+      <c r="F90" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="G90" s="36"/>
-      <c r="H90" s="36"/>
-      <c r="I90" s="36"/>
-      <c r="J90" s="36"/>
-      <c r="K90" s="36"/>
-      <c r="L90" s="36"/>
-      <c r="M90" s="36"/>
-      <c r="N90" s="36"/>
-      <c r="O90" s="36"/>
-      <c r="P90" s="35"/>
+      <c r="G90" s="30"/>
+      <c r="H90" s="30"/>
+      <c r="I90" s="30"/>
+      <c r="J90" s="30"/>
+      <c r="K90" s="30"/>
+      <c r="L90" s="30"/>
+      <c r="M90" s="30"/>
+      <c r="N90" s="30"/>
+      <c r="O90" s="30"/>
+      <c r="P90" s="29"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B91" s="37" t="s">
+      <c r="B91" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="C91" s="38" t="s">
+      <c r="C91" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="D91" s="38" t="s">
+      <c r="D91" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="E91" s="38" t="s">
+      <c r="E91" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="F91" s="38" t="s">
+      <c r="F91" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="G91" s="38"/>
-      <c r="H91" s="38"/>
-      <c r="I91" s="38"/>
-      <c r="J91" s="38"/>
-      <c r="K91" s="38"/>
-      <c r="L91" s="38"/>
-      <c r="M91" s="38"/>
-      <c r="N91" s="38"/>
-      <c r="O91" s="38"/>
-      <c r="P91" s="39"/>
+      <c r="G91" s="32"/>
+      <c r="H91" s="32"/>
+      <c r="I91" s="32"/>
+      <c r="J91" s="32"/>
+      <c r="K91" s="32"/>
+      <c r="L91" s="32"/>
+      <c r="M91" s="32"/>
+      <c r="N91" s="32"/>
+      <c r="O91" s="32"/>
+      <c r="P91" s="33"/>
     </row>
     <row r="92" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B92" s="37" t="s">
+      <c r="B92" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="C92" s="38" t="s">
+      <c r="C92" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="D92" s="38" t="s">
+      <c r="D92" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="E92" s="38" t="s">
+      <c r="E92" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="F92" s="38" t="s">
+      <c r="F92" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="G92" s="38"/>
-      <c r="H92" s="38"/>
-      <c r="I92" s="38"/>
-      <c r="J92" s="38"/>
-      <c r="K92" s="38"/>
-      <c r="L92" s="38"/>
-      <c r="M92" s="38"/>
-      <c r="N92" s="38"/>
-      <c r="O92" s="38"/>
-      <c r="P92" s="39"/>
+      <c r="G92" s="32"/>
+      <c r="H92" s="32"/>
+      <c r="I92" s="32"/>
+      <c r="J92" s="32"/>
+      <c r="K92" s="32"/>
+      <c r="L92" s="32"/>
+      <c r="M92" s="32"/>
+      <c r="N92" s="32"/>
+      <c r="O92" s="32"/>
+      <c r="P92" s="33"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B93" s="37" t="s">
+      <c r="B93" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="C93" s="38" t="s">
+      <c r="C93" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="D93" s="38" t="s">
+      <c r="D93" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E93" s="38" t="s">
+      <c r="E93" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="F93" s="38" t="s">
+      <c r="F93" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="G93" s="38"/>
-      <c r="H93" s="38"/>
-      <c r="I93" s="38"/>
-      <c r="J93" s="38"/>
-      <c r="K93" s="38"/>
-      <c r="L93" s="38"/>
-      <c r="M93" s="38"/>
-      <c r="N93" s="38"/>
-      <c r="O93" s="38"/>
-      <c r="P93" s="39"/>
+      <c r="G93" s="32"/>
+      <c r="H93" s="32"/>
+      <c r="I93" s="32"/>
+      <c r="J93" s="32"/>
+      <c r="K93" s="32"/>
+      <c r="L93" s="32"/>
+      <c r="M93" s="32"/>
+      <c r="N93" s="32"/>
+      <c r="O93" s="32"/>
+      <c r="P93" s="33"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B94" s="37" t="s">
+      <c r="B94" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="C94" s="38" t="s">
+      <c r="C94" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="D94" s="38" t="s">
+      <c r="D94" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E94" s="38" t="s">
+      <c r="E94" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="F94" s="38" t="s">
+      <c r="F94" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="G94" s="38"/>
-      <c r="H94" s="38"/>
-      <c r="I94" s="38"/>
-      <c r="J94" s="38"/>
-      <c r="K94" s="38"/>
-      <c r="L94" s="38"/>
-      <c r="M94" s="38"/>
-      <c r="N94" s="38"/>
-      <c r="O94" s="38"/>
-      <c r="P94" s="39"/>
+      <c r="G94" s="32"/>
+      <c r="H94" s="32"/>
+      <c r="I94" s="32"/>
+      <c r="J94" s="32"/>
+      <c r="K94" s="32"/>
+      <c r="L94" s="32"/>
+      <c r="M94" s="32"/>
+      <c r="N94" s="32"/>
+      <c r="O94" s="32"/>
+      <c r="P94" s="33"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B95" s="37" t="s">
+      <c r="B95" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="C95" s="38" t="s">
+      <c r="C95" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="D95" s="38" t="s">
+      <c r="D95" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="E95" s="38" t="s">
+      <c r="E95" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="F95" s="38" t="s">
+      <c r="F95" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="G95" s="38"/>
-      <c r="H95" s="38"/>
-      <c r="I95" s="38"/>
-      <c r="J95" s="38"/>
-      <c r="K95" s="38"/>
-      <c r="L95" s="38"/>
-      <c r="M95" s="38"/>
-      <c r="N95" s="38"/>
-      <c r="O95" s="38"/>
-      <c r="P95" s="39"/>
+      <c r="G95" s="32"/>
+      <c r="H95" s="32"/>
+      <c r="I95" s="32"/>
+      <c r="J95" s="32"/>
+      <c r="K95" s="32"/>
+      <c r="L95" s="32"/>
+      <c r="M95" s="32"/>
+      <c r="N95" s="32"/>
+      <c r="O95" s="32"/>
+      <c r="P95" s="33"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B96" s="37" t="s">
+      <c r="B96" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="C96" s="38" t="s">
+      <c r="C96" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="D96" s="38" t="s">
+      <c r="D96" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="E96" s="38" t="s">
+      <c r="E96" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="F96" s="38" t="s">
+      <c r="F96" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="G96" s="38"/>
-      <c r="H96" s="38"/>
-      <c r="I96" s="38"/>
-      <c r="J96" s="38"/>
-      <c r="K96" s="38"/>
-      <c r="L96" s="38"/>
-      <c r="M96" s="38"/>
-      <c r="N96" s="38"/>
-      <c r="O96" s="38"/>
-      <c r="P96" s="39"/>
+      <c r="G96" s="32"/>
+      <c r="H96" s="32"/>
+      <c r="I96" s="32"/>
+      <c r="J96" s="32"/>
+      <c r="K96" s="32"/>
+      <c r="L96" s="32"/>
+      <c r="M96" s="32"/>
+      <c r="N96" s="32"/>
+      <c r="O96" s="32"/>
+      <c r="P96" s="33"/>
     </row>
     <row r="97" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B97" s="37" t="s">
+      <c r="B97" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="C97" s="38" t="s">
+      <c r="C97" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="D97" s="38" t="s">
+      <c r="D97" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="E97" s="38" t="s">
+      <c r="E97" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="F97" s="38" t="s">
+      <c r="F97" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="G97" s="38"/>
-      <c r="H97" s="38"/>
-      <c r="I97" s="38"/>
-      <c r="J97" s="38"/>
-      <c r="K97" s="38"/>
-      <c r="L97" s="38"/>
-      <c r="M97" s="38"/>
-      <c r="N97" s="38"/>
-      <c r="O97" s="38"/>
-      <c r="P97" s="39"/>
+      <c r="G97" s="32"/>
+      <c r="H97" s="32"/>
+      <c r="I97" s="32"/>
+      <c r="J97" s="32"/>
+      <c r="K97" s="32"/>
+      <c r="L97" s="32"/>
+      <c r="M97" s="32"/>
+      <c r="N97" s="32"/>
+      <c r="O97" s="32"/>
+      <c r="P97" s="33"/>
     </row>
     <row r="98" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B98" s="37" t="s">
+      <c r="B98" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="C98" s="38" t="s">
+      <c r="C98" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="D98" s="38" t="s">
+      <c r="D98" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="E98" s="38" t="s">
+      <c r="E98" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="F98" s="38" t="s">
+      <c r="F98" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="G98" s="38"/>
-      <c r="H98" s="38"/>
-      <c r="I98" s="38"/>
-      <c r="J98" s="38"/>
-      <c r="K98" s="38"/>
-      <c r="L98" s="38"/>
-      <c r="M98" s="38"/>
-      <c r="N98" s="38"/>
-      <c r="O98" s="38"/>
-      <c r="P98" s="39"/>
+      <c r="G98" s="32"/>
+      <c r="H98" s="32"/>
+      <c r="I98" s="32"/>
+      <c r="J98" s="32"/>
+      <c r="K98" s="32"/>
+      <c r="L98" s="32"/>
+      <c r="M98" s="32"/>
+      <c r="N98" s="32"/>
+      <c r="O98" s="32"/>
+      <c r="P98" s="33"/>
     </row>
     <row r="99" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B99" s="37" t="s">
+      <c r="B99" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="C99" s="38" t="s">
+      <c r="C99" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="D99" s="38" t="s">
+      <c r="D99" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="E99" s="38" t="s">
+      <c r="E99" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="F99" s="38" t="s">
+      <c r="F99" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="G99" s="38"/>
-      <c r="H99" s="38"/>
-      <c r="I99" s="38"/>
-      <c r="J99" s="38"/>
-      <c r="K99" s="38"/>
-      <c r="L99" s="38"/>
-      <c r="M99" s="38"/>
-      <c r="N99" s="38"/>
-      <c r="O99" s="38"/>
-      <c r="P99" s="39"/>
+      <c r="G99" s="32"/>
+      <c r="H99" s="32"/>
+      <c r="I99" s="32"/>
+      <c r="J99" s="32"/>
+      <c r="K99" s="32"/>
+      <c r="L99" s="32"/>
+      <c r="M99" s="32"/>
+      <c r="N99" s="32"/>
+      <c r="O99" s="32"/>
+      <c r="P99" s="33"/>
     </row>
     <row r="100" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B100" s="37" t="s">
+      <c r="B100" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C100" s="38" t="s">
+      <c r="C100" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="D100" s="38" t="s">
+      <c r="D100" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E100" s="38" t="s">
+      <c r="E100" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="F100" s="38" t="s">
+      <c r="F100" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="G100" s="38"/>
-      <c r="H100" s="38"/>
-      <c r="I100" s="38"/>
-      <c r="J100" s="38"/>
-      <c r="K100" s="38"/>
-      <c r="L100" s="38"/>
-      <c r="M100" s="38"/>
-      <c r="N100" s="38"/>
-      <c r="O100" s="38"/>
-      <c r="P100" s="39"/>
+      <c r="G100" s="32"/>
+      <c r="H100" s="32"/>
+      <c r="I100" s="32"/>
+      <c r="J100" s="32"/>
+      <c r="K100" s="32"/>
+      <c r="L100" s="32"/>
+      <c r="M100" s="32"/>
+      <c r="N100" s="32"/>
+      <c r="O100" s="32"/>
+      <c r="P100" s="33"/>
     </row>
     <row r="101" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B101" s="37" t="s">
+      <c r="B101" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C101" s="38" t="s">
+      <c r="C101" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="D101" s="38" t="s">
+      <c r="D101" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="E101" s="38" t="s">
+      <c r="E101" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="F101" s="38" t="s">
+      <c r="F101" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="G101" s="38"/>
-      <c r="H101" s="38"/>
-      <c r="I101" s="38"/>
-      <c r="J101" s="38"/>
-      <c r="K101" s="38"/>
-      <c r="L101" s="38"/>
-      <c r="M101" s="38"/>
-      <c r="N101" s="38"/>
-      <c r="O101" s="38"/>
-      <c r="P101" s="39"/>
+      <c r="G101" s="32"/>
+      <c r="H101" s="32"/>
+      <c r="I101" s="32"/>
+      <c r="J101" s="32"/>
+      <c r="K101" s="32"/>
+      <c r="L101" s="32"/>
+      <c r="M101" s="32"/>
+      <c r="N101" s="32"/>
+      <c r="O101" s="32"/>
+      <c r="P101" s="33"/>
     </row>
     <row r="102" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B102" s="37" t="s">
+      <c r="B102" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C102" s="38" t="s">
+      <c r="C102" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="D102" s="38" t="s">
+      <c r="D102" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="E102" s="38" t="s">
+      <c r="E102" s="32" t="s">
         <v>225</v>
       </c>
-      <c r="F102" s="38" t="s">
+      <c r="F102" s="32" t="s">
         <v>226</v>
       </c>
-      <c r="G102" s="38"/>
-      <c r="H102" s="38"/>
-      <c r="I102" s="38"/>
-      <c r="J102" s="38"/>
-      <c r="K102" s="38"/>
-      <c r="L102" s="38"/>
-      <c r="M102" s="38"/>
-      <c r="N102" s="38"/>
-      <c r="O102" s="38"/>
-      <c r="P102" s="39"/>
+      <c r="G102" s="32"/>
+      <c r="H102" s="32"/>
+      <c r="I102" s="32"/>
+      <c r="J102" s="32"/>
+      <c r="K102" s="32"/>
+      <c r="L102" s="32"/>
+      <c r="M102" s="32"/>
+      <c r="N102" s="32"/>
+      <c r="O102" s="32"/>
+      <c r="P102" s="33"/>
     </row>
     <row r="103" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B103" s="37" t="s">
+      <c r="B103" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C103" s="38" t="s">
+      <c r="C103" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="D103" s="38" t="s">
+      <c r="D103" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="E103" s="38" t="s">
+      <c r="E103" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="F103" s="38" t="s">
+      <c r="F103" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="G103" s="38"/>
-      <c r="H103" s="38"/>
-      <c r="I103" s="38"/>
-      <c r="J103" s="38"/>
-      <c r="K103" s="38"/>
-      <c r="L103" s="38"/>
-      <c r="M103" s="38"/>
-      <c r="N103" s="38"/>
-      <c r="O103" s="38"/>
-      <c r="P103" s="39"/>
+      <c r="G103" s="32"/>
+      <c r="H103" s="32"/>
+      <c r="I103" s="32"/>
+      <c r="J103" s="32"/>
+      <c r="K103" s="32"/>
+      <c r="L103" s="32"/>
+      <c r="M103" s="32"/>
+      <c r="N103" s="32"/>
+      <c r="O103" s="32"/>
+      <c r="P103" s="33"/>
     </row>
     <row r="104" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B104" s="37" t="s">
+      <c r="B104" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C104" s="38" t="s">
+      <c r="C104" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="D104" s="38" t="s">
+      <c r="D104" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="E104" s="38" t="s">
+      <c r="E104" s="32" t="s">
         <v>232</v>
       </c>
-      <c r="F104" s="38" t="s">
+      <c r="F104" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="G104" s="38"/>
-      <c r="H104" s="38"/>
-      <c r="I104" s="38"/>
-      <c r="J104" s="38"/>
-      <c r="K104" s="38"/>
-      <c r="L104" s="38"/>
-      <c r="M104" s="38"/>
-      <c r="N104" s="38"/>
-      <c r="O104" s="38"/>
-      <c r="P104" s="39"/>
+      <c r="G104" s="32"/>
+      <c r="H104" s="32"/>
+      <c r="I104" s="32"/>
+      <c r="J104" s="32"/>
+      <c r="K104" s="32"/>
+      <c r="L104" s="32"/>
+      <c r="M104" s="32"/>
+      <c r="N104" s="32"/>
+      <c r="O104" s="32"/>
+      <c r="P104" s="33"/>
     </row>
     <row r="105" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B105" s="37" t="s">
+      <c r="B105" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C105" s="38" t="s">
+      <c r="C105" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="D105" s="38" t="s">
+      <c r="D105" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E105" s="38" t="s">
+      <c r="E105" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="F105" s="38" t="s">
+      <c r="F105" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="G105" s="38"/>
-      <c r="H105" s="38"/>
-      <c r="I105" s="38"/>
-      <c r="J105" s="38"/>
-      <c r="K105" s="38"/>
-      <c r="L105" s="38"/>
-      <c r="M105" s="38"/>
-      <c r="N105" s="38"/>
-      <c r="O105" s="38"/>
-      <c r="P105" s="39"/>
+      <c r="G105" s="32"/>
+      <c r="H105" s="32"/>
+      <c r="I105" s="32"/>
+      <c r="J105" s="32"/>
+      <c r="K105" s="32"/>
+      <c r="L105" s="32"/>
+      <c r="M105" s="32"/>
+      <c r="N105" s="32"/>
+      <c r="O105" s="32"/>
+      <c r="P105" s="33"/>
     </row>
     <row r="106" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B106" s="37" t="s">
+      <c r="B106" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C106" s="38" t="s">
+      <c r="C106" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="D106" s="38" t="s">
+      <c r="D106" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E106" s="38" t="s">
+      <c r="E106" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="F106" s="38" t="s">
+      <c r="F106" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="G106" s="38"/>
-      <c r="H106" s="38"/>
-      <c r="I106" s="38"/>
-      <c r="J106" s="38"/>
-      <c r="K106" s="38"/>
-      <c r="L106" s="38"/>
-      <c r="M106" s="38"/>
-      <c r="N106" s="38"/>
-      <c r="O106" s="38"/>
-      <c r="P106" s="39"/>
+      <c r="G106" s="32"/>
+      <c r="H106" s="32"/>
+      <c r="I106" s="32"/>
+      <c r="J106" s="32"/>
+      <c r="K106" s="32"/>
+      <c r="L106" s="32"/>
+      <c r="M106" s="32"/>
+      <c r="N106" s="32"/>
+      <c r="O106" s="32"/>
+      <c r="P106" s="33"/>
     </row>
     <row r="107" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B107" s="37" t="s">
+      <c r="B107" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C107" s="38" t="s">
+      <c r="C107" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="D107" s="38" t="s">
+      <c r="D107" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E107" s="38" t="s">
+      <c r="E107" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="F107" s="38" t="s">
+      <c r="F107" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="G107" s="38"/>
-      <c r="H107" s="38"/>
-      <c r="I107" s="38"/>
-      <c r="J107" s="38"/>
-      <c r="K107" s="38"/>
-      <c r="L107" s="38"/>
-      <c r="M107" s="38"/>
-      <c r="N107" s="38"/>
-      <c r="O107" s="38"/>
-      <c r="P107" s="39"/>
+      <c r="G107" s="32"/>
+      <c r="H107" s="32"/>
+      <c r="I107" s="32"/>
+      <c r="J107" s="32"/>
+      <c r="K107" s="32"/>
+      <c r="L107" s="32"/>
+      <c r="M107" s="32"/>
+      <c r="N107" s="32"/>
+      <c r="O107" s="32"/>
+      <c r="P107" s="33"/>
     </row>
     <row r="108" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B108" s="37" t="s">
+      <c r="B108" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C108" s="38" t="s">
+      <c r="C108" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="D108" s="38" t="s">
+      <c r="D108" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="E108" s="38" t="s">
+      <c r="E108" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="F108" s="38" t="s">
+      <c r="F108" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="G108" s="38"/>
-      <c r="H108" s="38"/>
-      <c r="I108" s="38"/>
-      <c r="J108" s="38"/>
-      <c r="K108" s="38"/>
-      <c r="L108" s="38"/>
-      <c r="M108" s="38"/>
-      <c r="N108" s="38"/>
-      <c r="O108" s="38"/>
-      <c r="P108" s="39"/>
+      <c r="G108" s="32"/>
+      <c r="H108" s="32"/>
+      <c r="I108" s="32"/>
+      <c r="J108" s="32"/>
+      <c r="K108" s="32"/>
+      <c r="L108" s="32"/>
+      <c r="M108" s="32"/>
+      <c r="N108" s="32"/>
+      <c r="O108" s="32"/>
+      <c r="P108" s="33"/>
     </row>
     <row r="109" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B109" s="37" t="s">
+      <c r="B109" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C109" s="38" t="s">
+      <c r="C109" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="D109" s="38" t="s">
+      <c r="D109" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="E109" s="38" t="s">
+      <c r="E109" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="F109" s="38" t="s">
+      <c r="F109" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="G109" s="38"/>
-      <c r="H109" s="38"/>
-      <c r="I109" s="38"/>
-      <c r="J109" s="38"/>
-      <c r="K109" s="38"/>
-      <c r="L109" s="38"/>
-      <c r="M109" s="38"/>
-      <c r="N109" s="38"/>
-      <c r="O109" s="38"/>
-      <c r="P109" s="39"/>
+      <c r="G109" s="32"/>
+      <c r="H109" s="32"/>
+      <c r="I109" s="32"/>
+      <c r="J109" s="32"/>
+      <c r="K109" s="32"/>
+      <c r="L109" s="32"/>
+      <c r="M109" s="32"/>
+      <c r="N109" s="32"/>
+      <c r="O109" s="32"/>
+      <c r="P109" s="33"/>
     </row>
     <row r="110" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B110" s="37" t="s">
+      <c r="B110" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C110" s="38" t="s">
+      <c r="C110" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D110" s="38" t="s">
+      <c r="D110" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="E110" s="38" t="s">
+      <c r="E110" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="F110" s="38" t="s">
+      <c r="F110" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="G110" s="38"/>
-      <c r="H110" s="38"/>
-      <c r="I110" s="38"/>
-      <c r="J110" s="38"/>
-      <c r="K110" s="38"/>
-      <c r="L110" s="38"/>
-      <c r="M110" s="38"/>
-      <c r="N110" s="38"/>
-      <c r="O110" s="38"/>
-      <c r="P110" s="39"/>
+      <c r="G110" s="32"/>
+      <c r="H110" s="32"/>
+      <c r="I110" s="32"/>
+      <c r="J110" s="32"/>
+      <c r="K110" s="32"/>
+      <c r="L110" s="32"/>
+      <c r="M110" s="32"/>
+      <c r="N110" s="32"/>
+      <c r="O110" s="32"/>
+      <c r="P110" s="33"/>
     </row>
     <row r="111" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B111" s="37" t="s">
+      <c r="B111" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C111" s="38" t="s">
+      <c r="C111" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="D111" s="38" t="s">
+      <c r="D111" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="E111" s="38" t="s">
+      <c r="E111" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="F111" s="38" t="s">
+      <c r="F111" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="G111" s="38"/>
-      <c r="H111" s="38"/>
-      <c r="I111" s="38"/>
-      <c r="J111" s="38"/>
-      <c r="K111" s="38"/>
-      <c r="L111" s="38"/>
-      <c r="M111" s="38"/>
-      <c r="N111" s="38"/>
-      <c r="O111" s="38"/>
-      <c r="P111" s="39"/>
+      <c r="G111" s="32"/>
+      <c r="H111" s="32"/>
+      <c r="I111" s="32"/>
+      <c r="J111" s="32"/>
+      <c r="K111" s="32"/>
+      <c r="L111" s="32"/>
+      <c r="M111" s="32"/>
+      <c r="N111" s="32"/>
+      <c r="O111" s="32"/>
+      <c r="P111" s="33"/>
     </row>
     <row r="112" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B112" s="37" t="s">
+      <c r="B112" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C112" s="38" t="s">
+      <c r="C112" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="D112" s="38" t="s">
+      <c r="D112" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="E112" s="38" t="s">
+      <c r="E112" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="F112" s="38" t="s">
+      <c r="F112" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="G112" s="38"/>
-      <c r="H112" s="38"/>
-      <c r="I112" s="38"/>
-      <c r="J112" s="38"/>
-      <c r="K112" s="38"/>
-      <c r="L112" s="38"/>
-      <c r="M112" s="38"/>
-      <c r="N112" s="38"/>
-      <c r="O112" s="38"/>
-      <c r="P112" s="39"/>
+      <c r="G112" s="32"/>
+      <c r="H112" s="32"/>
+      <c r="I112" s="32"/>
+      <c r="J112" s="32"/>
+      <c r="K112" s="32"/>
+      <c r="L112" s="32"/>
+      <c r="M112" s="32"/>
+      <c r="N112" s="32"/>
+      <c r="O112" s="32"/>
+      <c r="P112" s="33"/>
     </row>
     <row r="113" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B113" s="37" t="s">
+      <c r="B113" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C113" s="38" t="s">
+      <c r="C113" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="D113" s="38" t="s">
+      <c r="D113" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E113" s="38" t="s">
+      <c r="E113" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="F113" s="38" t="s">
+      <c r="F113" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="G113" s="38"/>
-      <c r="H113" s="38"/>
-      <c r="I113" s="38"/>
-      <c r="J113" s="38"/>
-      <c r="K113" s="38"/>
-      <c r="L113" s="38"/>
-      <c r="M113" s="38"/>
-      <c r="N113" s="38"/>
-      <c r="O113" s="38"/>
-      <c r="P113" s="39"/>
+      <c r="G113" s="32"/>
+      <c r="H113" s="32"/>
+      <c r="I113" s="32"/>
+      <c r="J113" s="32"/>
+      <c r="K113" s="32"/>
+      <c r="L113" s="32"/>
+      <c r="M113" s="32"/>
+      <c r="N113" s="32"/>
+      <c r="O113" s="32"/>
+      <c r="P113" s="33"/>
     </row>
     <row r="114" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B114" s="37" t="s">
+      <c r="B114" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C114" s="38" t="s">
+      <c r="C114" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="D114" s="38" t="s">
+      <c r="D114" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="E114" s="38" t="s">
+      <c r="E114" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="F114" s="38" t="s">
+      <c r="F114" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="G114" s="38"/>
-      <c r="H114" s="38"/>
-      <c r="I114" s="38"/>
-      <c r="J114" s="38"/>
-      <c r="K114" s="38"/>
-      <c r="L114" s="38"/>
-      <c r="M114" s="38"/>
-      <c r="N114" s="38"/>
-      <c r="O114" s="38"/>
-      <c r="P114" s="39"/>
+      <c r="G114" s="32"/>
+      <c r="H114" s="32"/>
+      <c r="I114" s="32"/>
+      <c r="J114" s="32"/>
+      <c r="K114" s="32"/>
+      <c r="L114" s="32"/>
+      <c r="M114" s="32"/>
+      <c r="N114" s="32"/>
+      <c r="O114" s="32"/>
+      <c r="P114" s="33"/>
     </row>
     <row r="115" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B115" s="37" t="s">
+      <c r="B115" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="C115" s="38" t="s">
+      <c r="C115" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="D115" s="38" t="s">
+      <c r="D115" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="E115" s="38" t="s">
+      <c r="E115" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="F115" s="38" t="s">
+      <c r="F115" s="32" t="s">
         <v>269</v>
       </c>
-      <c r="G115" s="38"/>
-      <c r="H115" s="38"/>
-      <c r="I115" s="38"/>
-      <c r="J115" s="38"/>
-      <c r="K115" s="38"/>
-      <c r="L115" s="38"/>
-      <c r="M115" s="39"/>
+      <c r="G115" s="32"/>
+      <c r="H115" s="32"/>
+      <c r="I115" s="32"/>
+      <c r="J115" s="32"/>
+      <c r="K115" s="32"/>
+      <c r="L115" s="32"/>
+      <c r="M115" s="33"/>
     </row>
     <row r="116" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B116" s="37" t="s">
+      <c r="B116" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="C116" s="38" t="s">
+      <c r="C116" s="32" t="s">
         <v>270</v>
       </c>
-      <c r="D116" s="38" t="s">
+      <c r="D116" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="E116" s="38" t="s">
+      <c r="E116" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="F116" s="38" t="s">
+      <c r="F116" s="32" t="s">
         <v>273</v>
       </c>
-      <c r="G116" s="38"/>
-      <c r="H116" s="38"/>
-      <c r="I116" s="38"/>
-      <c r="J116" s="38"/>
-      <c r="K116" s="38"/>
-      <c r="L116" s="38"/>
-      <c r="M116" s="39"/>
+      <c r="G116" s="32"/>
+      <c r="H116" s="32"/>
+      <c r="I116" s="32"/>
+      <c r="J116" s="32"/>
+      <c r="K116" s="32"/>
+      <c r="L116" s="32"/>
+      <c r="M116" s="33"/>
     </row>
     <row r="117" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B117" s="37" t="s">
+      <c r="B117" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="C117" s="38" t="s">
+      <c r="C117" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="D117" s="38" t="s">
+      <c r="D117" s="32" t="s">
         <v>275</v>
       </c>
-      <c r="E117" s="38" t="s">
+      <c r="E117" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="F117" s="38" t="s">
+      <c r="F117" s="32" t="s">
         <v>277</v>
       </c>
-      <c r="G117" s="38"/>
-      <c r="H117" s="38"/>
-      <c r="I117" s="38"/>
-      <c r="J117" s="38"/>
-      <c r="K117" s="38"/>
-      <c r="L117" s="38"/>
-      <c r="M117" s="39"/>
+      <c r="G117" s="32"/>
+      <c r="H117" s="32"/>
+      <c r="I117" s="32"/>
+      <c r="J117" s="32"/>
+      <c r="K117" s="32"/>
+      <c r="L117" s="32"/>
+      <c r="M117" s="33"/>
     </row>
     <row r="118" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B118" s="37" t="s">
+      <c r="B118" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="C118" s="38" t="s">
+      <c r="C118" s="32" t="s">
         <v>278</v>
       </c>
-      <c r="D118" s="38" t="s">
+      <c r="D118" s="32" t="s">
         <v>279</v>
       </c>
-      <c r="E118" s="38" t="s">
+      <c r="E118" s="32" t="s">
         <v>280</v>
       </c>
-      <c r="F118" s="38" t="s">
+      <c r="F118" s="32" t="s">
         <v>281</v>
       </c>
-      <c r="G118" s="38"/>
-      <c r="H118" s="38"/>
-      <c r="I118" s="38"/>
-      <c r="J118" s="38"/>
-      <c r="K118" s="38"/>
-      <c r="L118" s="38"/>
-      <c r="M118" s="39"/>
+      <c r="G118" s="32"/>
+      <c r="H118" s="32"/>
+      <c r="I118" s="32"/>
+      <c r="J118" s="32"/>
+      <c r="K118" s="32"/>
+      <c r="L118" s="32"/>
+      <c r="M118" s="33"/>
     </row>
     <row r="119" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B119" s="37" t="s">
+      <c r="B119" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="C119" s="38" t="s">
+      <c r="C119" s="32" t="s">
         <v>282</v>
       </c>
-      <c r="D119" s="38" t="s">
+      <c r="D119" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="E119" s="38" t="s">
+      <c r="E119" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="F119" s="38" t="s">
+      <c r="F119" s="32" t="s">
         <v>285</v>
       </c>
-      <c r="G119" s="38"/>
-      <c r="H119" s="38"/>
-      <c r="I119" s="38"/>
-      <c r="J119" s="38"/>
-      <c r="K119" s="38"/>
-      <c r="L119" s="38"/>
-      <c r="M119" s="39"/>
+      <c r="G119" s="32"/>
+      <c r="H119" s="32"/>
+      <c r="I119" s="32"/>
+      <c r="J119" s="32"/>
+      <c r="K119" s="32"/>
+      <c r="L119" s="32"/>
+      <c r="M119" s="33"/>
     </row>
     <row r="120" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B120" s="37" t="s">
+      <c r="B120" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="C120" s="38" t="s">
+      <c r="C120" s="32" t="s">
         <v>286</v>
       </c>
-      <c r="D120" s="38" t="s">
+      <c r="D120" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="E120" s="38" t="s">
+      <c r="E120" s="32" t="s">
         <v>287</v>
       </c>
-      <c r="F120" s="38" t="s">
+      <c r="F120" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="G120" s="38"/>
-      <c r="H120" s="38"/>
-      <c r="I120" s="38"/>
-      <c r="J120" s="38"/>
-      <c r="K120" s="38"/>
-      <c r="L120" s="38"/>
-      <c r="M120" s="39"/>
+      <c r="G120" s="32"/>
+      <c r="H120" s="32"/>
+      <c r="I120" s="32"/>
+      <c r="J120" s="32"/>
+      <c r="K120" s="32"/>
+      <c r="L120" s="32"/>
+      <c r="M120" s="33"/>
     </row>
     <row r="121" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B121" s="37" t="s">
+      <c r="B121" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="C121" s="38" t="s">
+      <c r="C121" s="32" t="s">
         <v>289</v>
       </c>
-      <c r="D121" s="38" t="s">
+      <c r="D121" s="32" t="s">
         <v>290</v>
       </c>
-      <c r="E121" s="38" t="s">
+      <c r="E121" s="32" t="s">
         <v>291</v>
       </c>
-      <c r="F121" s="38" t="s">
+      <c r="F121" s="32" t="s">
         <v>292</v>
       </c>
-      <c r="G121" s="38"/>
-      <c r="H121" s="38"/>
-      <c r="I121" s="38"/>
-      <c r="J121" s="38"/>
-      <c r="K121" s="38"/>
-      <c r="L121" s="38"/>
-      <c r="M121" s="39"/>
+      <c r="G121" s="32"/>
+      <c r="H121" s="32"/>
+      <c r="I121" s="32"/>
+      <c r="J121" s="32"/>
+      <c r="K121" s="32"/>
+      <c r="L121" s="32"/>
+      <c r="M121" s="33"/>
     </row>
     <row r="122" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B122" s="37" t="s">
+      <c r="B122" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="C122" s="38" t="s">
+      <c r="C122" s="32" t="s">
         <v>293</v>
       </c>
-      <c r="D122" s="38" t="s">
+      <c r="D122" s="32" t="s">
         <v>294</v>
       </c>
-      <c r="E122" s="38" t="s">
+      <c r="E122" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="F122" s="38" t="s">
+      <c r="F122" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="G122" s="38"/>
-      <c r="H122" s="38"/>
-      <c r="I122" s="38"/>
-      <c r="J122" s="38"/>
-      <c r="K122" s="38"/>
-      <c r="L122" s="38"/>
-      <c r="M122" s="39"/>
+      <c r="G122" s="32"/>
+      <c r="H122" s="32"/>
+      <c r="I122" s="32"/>
+      <c r="J122" s="32"/>
+      <c r="K122" s="32"/>
+      <c r="L122" s="32"/>
+      <c r="M122" s="33"/>
     </row>
     <row r="123" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B123" s="37" t="s">
+      <c r="B123" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="C123" s="38" t="s">
+      <c r="C123" s="32" t="s">
         <v>297</v>
       </c>
-      <c r="D123" s="38" t="s">
+      <c r="D123" s="32" t="s">
         <v>298</v>
       </c>
-      <c r="E123" s="38" t="s">
+      <c r="E123" s="32" t="s">
         <v>299</v>
       </c>
-      <c r="F123" s="38" t="s">
+      <c r="F123" s="32" t="s">
         <v>300</v>
       </c>
-      <c r="G123" s="38"/>
-      <c r="H123" s="38"/>
-      <c r="I123" s="38"/>
-      <c r="J123" s="38"/>
-      <c r="K123" s="38"/>
-      <c r="L123" s="38"/>
-      <c r="M123" s="39"/>
+      <c r="G123" s="32"/>
+      <c r="H123" s="32"/>
+      <c r="I123" s="32"/>
+      <c r="J123" s="32"/>
+      <c r="K123" s="32"/>
+      <c r="L123" s="32"/>
+      <c r="M123" s="33"/>
     </row>
     <row r="124" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B124" s="37" t="s">
+      <c r="B124" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="C124" s="38" t="s">
+      <c r="C124" s="32" t="s">
         <v>301</v>
       </c>
-      <c r="D124" s="38" t="s">
+      <c r="D124" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="E124" s="38" t="s">
+      <c r="E124" s="32" t="s">
         <v>303</v>
       </c>
-      <c r="F124" s="38" t="s">
+      <c r="F124" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="G124" s="38"/>
-      <c r="H124" s="38"/>
-      <c r="I124" s="38"/>
-      <c r="J124" s="38"/>
-      <c r="K124" s="38"/>
-      <c r="L124" s="38"/>
-      <c r="M124" s="39"/>
+      <c r="G124" s="32"/>
+      <c r="H124" s="32"/>
+      <c r="I124" s="32"/>
+      <c r="J124" s="32"/>
+      <c r="K124" s="32"/>
+      <c r="L124" s="32"/>
+      <c r="M124" s="33"/>
     </row>
     <row r="125" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B125" s="37" t="s">
+      <c r="B125" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="C125" s="38" t="s">
+      <c r="C125" s="32" t="s">
         <v>305</v>
       </c>
-      <c r="D125" s="38" t="s">
+      <c r="D125" s="32" t="s">
         <v>306</v>
       </c>
-      <c r="E125" s="38" t="s">
+      <c r="E125" s="32" t="s">
         <v>307</v>
       </c>
-      <c r="F125" s="38" t="s">
+      <c r="F125" s="32" t="s">
         <v>308</v>
       </c>
-      <c r="G125" s="38"/>
-      <c r="H125" s="38"/>
-      <c r="I125" s="38"/>
-      <c r="J125" s="38"/>
-      <c r="K125" s="38"/>
-      <c r="L125" s="38"/>
-      <c r="M125" s="39"/>
+      <c r="G125" s="32"/>
+      <c r="H125" s="32"/>
+      <c r="I125" s="32"/>
+      <c r="J125" s="32"/>
+      <c r="K125" s="32"/>
+      <c r="L125" s="32"/>
+      <c r="M125" s="33"/>
     </row>
     <row r="126" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B126" s="37" t="s">
+      <c r="B126" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C126" s="38" t="s">
+      <c r="C126" s="32" t="s">
         <v>309</v>
       </c>
-      <c r="D126" s="38" t="s">
+      <c r="D126" s="32" t="s">
         <v>310</v>
       </c>
-      <c r="E126" s="38" t="s">
+      <c r="E126" s="32" t="s">
         <v>311</v>
       </c>
-      <c r="F126" s="38" t="s">
+      <c r="F126" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="G126" s="38"/>
-      <c r="H126" s="38"/>
-      <c r="I126" s="38"/>
-      <c r="J126" s="38"/>
-      <c r="K126" s="38"/>
-      <c r="L126" s="38"/>
-      <c r="M126" s="39"/>
+      <c r="G126" s="32"/>
+      <c r="H126" s="32"/>
+      <c r="I126" s="32"/>
+      <c r="J126" s="32"/>
+      <c r="K126" s="32"/>
+      <c r="L126" s="32"/>
+      <c r="M126" s="33"/>
     </row>
     <row r="127" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B127" s="37" t="s">
+      <c r="B127" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="C127" s="38" t="s">
+      <c r="C127" s="32" t="s">
         <v>313</v>
       </c>
-      <c r="D127" s="38" t="s">
+      <c r="D127" s="32" t="s">
         <v>314</v>
       </c>
-      <c r="E127" s="38" t="s">
+      <c r="E127" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="F127" s="38" t="s">
+      <c r="F127" s="32" t="s">
         <v>316</v>
       </c>
-      <c r="G127" s="38"/>
-      <c r="H127" s="38"/>
-      <c r="I127" s="38"/>
-      <c r="J127" s="38"/>
-      <c r="K127" s="38"/>
-      <c r="L127" s="38"/>
-      <c r="M127" s="39"/>
+      <c r="G127" s="32"/>
+      <c r="H127" s="32"/>
+      <c r="I127" s="32"/>
+      <c r="J127" s="32"/>
+      <c r="K127" s="32"/>
+      <c r="L127" s="32"/>
+      <c r="M127" s="33"/>
     </row>
     <row r="128" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B128" s="37" t="s">
+      <c r="B128" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="C128" s="38" t="s">
+      <c r="C128" s="32" t="s">
         <v>317</v>
       </c>
-      <c r="D128" s="38" t="s">
+      <c r="D128" s="32" t="s">
         <v>318</v>
       </c>
-      <c r="E128" s="38" t="s">
+      <c r="E128" s="32" t="s">
         <v>319</v>
       </c>
-      <c r="F128" s="38" t="s">
+      <c r="F128" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="G128" s="38"/>
-      <c r="H128" s="38"/>
-      <c r="I128" s="38"/>
-      <c r="J128" s="38"/>
-      <c r="K128" s="38"/>
-      <c r="L128" s="38"/>
-      <c r="M128" s="39"/>
+      <c r="G128" s="32"/>
+      <c r="H128" s="32"/>
+      <c r="I128" s="32"/>
+      <c r="J128" s="32"/>
+      <c r="K128" s="32"/>
+      <c r="L128" s="32"/>
+      <c r="M128" s="33"/>
     </row>
     <row r="129" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B129" s="37" t="s">
+      <c r="B129" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="C129" s="38" t="s">
+      <c r="C129" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="D129" s="38" t="s">
+      <c r="D129" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="E129" s="38" t="s">
+      <c r="E129" s="32" t="s">
         <v>323</v>
       </c>
-      <c r="F129" s="38" t="s">
+      <c r="F129" s="32" t="s">
         <v>324</v>
       </c>
-      <c r="G129" s="38"/>
-      <c r="H129" s="38"/>
-      <c r="I129" s="38"/>
-      <c r="J129" s="38"/>
-      <c r="K129" s="38"/>
-      <c r="L129" s="38"/>
-      <c r="M129" s="39"/>
+      <c r="G129" s="32"/>
+      <c r="H129" s="32"/>
+      <c r="I129" s="32"/>
+      <c r="J129" s="32"/>
+      <c r="K129" s="32"/>
+      <c r="L129" s="32"/>
+      <c r="M129" s="33"/>
     </row>
     <row r="130" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B130" s="37" t="s">
+      <c r="B130" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="C130" s="38" t="s">
+      <c r="C130" s="32" t="s">
         <v>325</v>
       </c>
-      <c r="D130" s="38" t="s">
+      <c r="D130" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="E130" s="38" t="s">
+      <c r="E130" s="32" t="s">
         <v>327</v>
       </c>
-      <c r="F130" s="38" t="s">
+      <c r="F130" s="32" t="s">
         <v>328</v>
       </c>
-      <c r="G130" s="38"/>
-      <c r="H130" s="38"/>
-      <c r="I130" s="38"/>
-      <c r="J130" s="38"/>
-      <c r="K130" s="38"/>
-      <c r="L130" s="38"/>
-      <c r="M130" s="39"/>
+      <c r="G130" s="32"/>
+      <c r="H130" s="32"/>
+      <c r="I130" s="32"/>
+      <c r="J130" s="32"/>
+      <c r="K130" s="32"/>
+      <c r="L130" s="32"/>
+      <c r="M130" s="33"/>
     </row>
     <row r="131" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B131" s="37" t="s">
+      <c r="B131" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="C131" s="38" t="s">
+      <c r="C131" s="32" t="s">
         <v>329</v>
       </c>
-      <c r="D131" s="38" t="s">
+      <c r="D131" s="32" t="s">
         <v>330</v>
       </c>
-      <c r="E131" s="38" t="s">
+      <c r="E131" s="32" t="s">
         <v>331</v>
       </c>
-      <c r="F131" s="38" t="s">
+      <c r="F131" s="32" t="s">
         <v>332</v>
       </c>
-      <c r="G131" s="38"/>
-      <c r="H131" s="38"/>
-      <c r="I131" s="38"/>
-      <c r="J131" s="38"/>
-      <c r="K131" s="38"/>
-      <c r="L131" s="38"/>
-      <c r="M131" s="39"/>
+      <c r="G131" s="32"/>
+      <c r="H131" s="32"/>
+      <c r="I131" s="32"/>
+      <c r="J131" s="32"/>
+      <c r="K131" s="32"/>
+      <c r="L131" s="32"/>
+      <c r="M131" s="33"/>
     </row>
     <row r="132" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B132" s="37" t="s">
+      <c r="B132" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="C132" s="38" t="s">
+      <c r="C132" s="32" t="s">
         <v>333</v>
       </c>
-      <c r="D132" s="38" t="s">
+      <c r="D132" s="32" t="s">
         <v>334</v>
       </c>
-      <c r="E132" s="38" t="s">
+      <c r="E132" s="32" t="s">
         <v>335</v>
       </c>
-      <c r="F132" s="38" t="s">
+      <c r="F132" s="32" t="s">
         <v>336</v>
       </c>
-      <c r="G132" s="38"/>
-      <c r="H132" s="38"/>
-      <c r="I132" s="38"/>
-      <c r="J132" s="38"/>
-      <c r="K132" s="38"/>
-      <c r="L132" s="38"/>
-      <c r="M132" s="39"/>
+      <c r="G132" s="32"/>
+      <c r="H132" s="32"/>
+      <c r="I132" s="32"/>
+      <c r="J132" s="32"/>
+      <c r="K132" s="32"/>
+      <c r="L132" s="32"/>
+      <c r="M132" s="33"/>
     </row>
     <row r="133" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B133" s="37" t="s">
+      <c r="B133" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="C133" s="38" t="s">
+      <c r="C133" s="32" t="s">
         <v>337</v>
       </c>
-      <c r="D133" s="38" t="s">
+      <c r="D133" s="32" t="s">
         <v>338</v>
       </c>
-      <c r="E133" s="38" t="s">
+      <c r="E133" s="32" t="s">
         <v>339</v>
       </c>
-      <c r="F133" s="38" t="s">
+      <c r="F133" s="32" t="s">
         <v>340</v>
       </c>
-      <c r="G133" s="38"/>
-      <c r="H133" s="38"/>
-      <c r="I133" s="38"/>
-      <c r="J133" s="38"/>
-      <c r="K133" s="38"/>
-      <c r="L133" s="38"/>
-      <c r="M133" s="39"/>
+      <c r="G133" s="32"/>
+      <c r="H133" s="32"/>
+      <c r="I133" s="32"/>
+      <c r="J133" s="32"/>
+      <c r="K133" s="32"/>
+      <c r="L133" s="32"/>
+      <c r="M133" s="33"/>
     </row>
     <row r="134" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B134" s="37" t="s">
+      <c r="B134" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="C134" s="38" t="s">
+      <c r="C134" s="32" t="s">
         <v>341</v>
       </c>
-      <c r="D134" s="38" t="s">
+      <c r="D134" s="32" t="s">
         <v>342</v>
       </c>
-      <c r="E134" s="38" t="s">
+      <c r="E134" s="32" t="s">
         <v>343</v>
       </c>
-      <c r="F134" s="38" t="s">
+      <c r="F134" s="32" t="s">
         <v>344</v>
       </c>
-      <c r="G134" s="38"/>
-      <c r="H134" s="38"/>
-      <c r="I134" s="38"/>
-      <c r="J134" s="38"/>
-      <c r="K134" s="38"/>
-      <c r="L134" s="38"/>
-      <c r="M134" s="39"/>
+      <c r="G134" s="32"/>
+      <c r="H134" s="32"/>
+      <c r="I134" s="32"/>
+      <c r="J134" s="32"/>
+      <c r="K134" s="32"/>
+      <c r="L134" s="32"/>
+      <c r="M134" s="33"/>
     </row>
     <row r="135" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B135" s="37" t="s">
+      <c r="B135" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C135" s="38" t="s">
+      <c r="C135" s="32" t="s">
         <v>345</v>
       </c>
-      <c r="D135" s="38" t="s">
+      <c r="D135" s="32" t="s">
         <v>346</v>
       </c>
-      <c r="E135" s="38" t="s">
+      <c r="E135" s="32" t="s">
         <v>347</v>
       </c>
-      <c r="F135" s="38" t="s">
+      <c r="F135" s="32" t="s">
         <v>348</v>
       </c>
-      <c r="G135" s="38"/>
-      <c r="H135" s="38"/>
-      <c r="I135" s="38"/>
-      <c r="J135" s="38"/>
-      <c r="K135" s="38"/>
-      <c r="L135" s="38"/>
-      <c r="M135" s="39"/>
+      <c r="G135" s="32"/>
+      <c r="H135" s="32"/>
+      <c r="I135" s="32"/>
+      <c r="J135" s="32"/>
+      <c r="K135" s="32"/>
+      <c r="L135" s="32"/>
+      <c r="M135" s="33"/>
     </row>
     <row r="136" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B136" s="37" t="s">
+      <c r="B136" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="C136" s="38" t="s">
+      <c r="C136" s="32" t="s">
         <v>349</v>
       </c>
-      <c r="D136" s="38" t="s">
+      <c r="D136" s="32" t="s">
         <v>350</v>
       </c>
-      <c r="E136" s="38" t="s">
+      <c r="E136" s="32" t="s">
         <v>351</v>
       </c>
-      <c r="F136" s="38" t="s">
+      <c r="F136" s="32" t="s">
         <v>352</v>
       </c>
-      <c r="G136" s="38"/>
-      <c r="H136" s="38"/>
-      <c r="I136" s="38"/>
-      <c r="J136" s="38"/>
-      <c r="K136" s="38"/>
-      <c r="L136" s="38"/>
-      <c r="M136" s="39"/>
+      <c r="G136" s="32"/>
+      <c r="H136" s="32"/>
+      <c r="I136" s="32"/>
+      <c r="J136" s="32"/>
+      <c r="K136" s="32"/>
+      <c r="L136" s="32"/>
+      <c r="M136" s="33"/>
     </row>
     <row r="137" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B137" s="37" t="s">
+      <c r="B137" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="C137" s="38" t="s">
+      <c r="C137" s="32" t="s">
         <v>353</v>
       </c>
-      <c r="D137" s="38" t="s">
+      <c r="D137" s="32" t="s">
         <v>354</v>
       </c>
-      <c r="E137" s="38" t="s">
+      <c r="E137" s="32" t="s">
         <v>355</v>
       </c>
-      <c r="F137" s="38" t="s">
+      <c r="F137" s="32" t="s">
         <v>356</v>
       </c>
-      <c r="G137" s="38"/>
-      <c r="H137" s="38"/>
-      <c r="I137" s="38"/>
-      <c r="J137" s="38"/>
-      <c r="K137" s="38"/>
-      <c r="L137" s="38"/>
-      <c r="M137" s="39"/>
+      <c r="G137" s="32"/>
+      <c r="H137" s="32"/>
+      <c r="I137" s="32"/>
+      <c r="J137" s="32"/>
+      <c r="K137" s="32"/>
+      <c r="L137" s="32"/>
+      <c r="M137" s="33"/>
     </row>
     <row r="138" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B138" s="37" t="s">
+      <c r="B138" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="C138" s="38" t="s">
+      <c r="C138" s="32" t="s">
         <v>357</v>
       </c>
-      <c r="D138" s="38" t="s">
+      <c r="D138" s="32" t="s">
         <v>358</v>
       </c>
-      <c r="E138" s="38" t="s">
+      <c r="E138" s="32" t="s">
         <v>359</v>
       </c>
-      <c r="F138" s="38" t="s">
+      <c r="F138" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="G138" s="38"/>
-      <c r="H138" s="38"/>
-      <c r="I138" s="38"/>
-      <c r="J138" s="38"/>
-      <c r="K138" s="38"/>
-      <c r="L138" s="38"/>
-      <c r="M138" s="39"/>
+      <c r="G138" s="32"/>
+      <c r="H138" s="32"/>
+      <c r="I138" s="32"/>
+      <c r="J138" s="32"/>
+      <c r="K138" s="32"/>
+      <c r="L138" s="32"/>
+      <c r="M138" s="33"/>
     </row>
     <row r="139" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B139" s="37" t="s">
+      <c r="B139" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="C139" s="38" t="s">
+      <c r="C139" s="32" t="s">
         <v>361</v>
       </c>
-      <c r="D139" s="38" t="s">
+      <c r="D139" s="32" t="s">
         <v>362</v>
       </c>
-      <c r="E139" s="38" t="s">
+      <c r="E139" s="32" t="s">
         <v>363</v>
       </c>
-      <c r="F139" s="38" t="s">
+      <c r="F139" s="32" t="s">
         <v>364</v>
       </c>
-      <c r="G139" s="38"/>
-      <c r="H139" s="38"/>
-      <c r="I139" s="38"/>
-      <c r="J139" s="38"/>
-      <c r="K139" s="38"/>
-      <c r="L139" s="38"/>
-      <c r="M139" s="39"/>
+      <c r="G139" s="32"/>
+      <c r="H139" s="32"/>
+      <c r="I139" s="32"/>
+      <c r="J139" s="32"/>
+      <c r="K139" s="32"/>
+      <c r="L139" s="32"/>
+      <c r="M139" s="33"/>
     </row>
     <row r="140" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B140" s="37" t="s">
+      <c r="B140" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="C140" s="38" t="s">
+      <c r="C140" s="32" t="s">
         <v>365</v>
       </c>
-      <c r="D140" s="38" t="s">
+      <c r="D140" s="32" t="s">
         <v>366</v>
       </c>
-      <c r="E140" s="38" t="s">
+      <c r="E140" s="32" t="s">
         <v>367</v>
       </c>
-      <c r="F140" s="38" t="s">
+      <c r="F140" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="G140" s="38"/>
-      <c r="H140" s="38"/>
-      <c r="I140" s="38"/>
-      <c r="J140" s="38"/>
-      <c r="K140" s="38"/>
-      <c r="L140" s="38"/>
-      <c r="M140" s="39"/>
+      <c r="G140" s="32"/>
+      <c r="H140" s="32"/>
+      <c r="I140" s="32"/>
+      <c r="J140" s="32"/>
+      <c r="K140" s="32"/>
+      <c r="L140" s="32"/>
+      <c r="M140" s="33"/>
     </row>
     <row r="141" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B141" s="37" t="s">
+      <c r="B141" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="C141" s="38" t="s">
+      <c r="C141" s="32" t="s">
         <v>369</v>
       </c>
-      <c r="D141" s="38" t="s">
+      <c r="D141" s="32" t="s">
         <v>370</v>
       </c>
-      <c r="E141" s="38" t="s">
+      <c r="E141" s="32" t="s">
         <v>371</v>
       </c>
-      <c r="F141" s="38" t="s">
+      <c r="F141" s="32" t="s">
         <v>372</v>
       </c>
-      <c r="G141" s="38"/>
-      <c r="H141" s="38"/>
-      <c r="I141" s="38"/>
-      <c r="J141" s="38"/>
-      <c r="K141" s="38"/>
-      <c r="L141" s="38"/>
-      <c r="M141" s="39"/>
+      <c r="G141" s="32"/>
+      <c r="H141" s="32"/>
+      <c r="I141" s="32"/>
+      <c r="J141" s="32"/>
+      <c r="K141" s="32"/>
+      <c r="L141" s="32"/>
+      <c r="M141" s="33"/>
     </row>
     <row r="142" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B142" s="37" t="s">
+      <c r="B142" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C142" s="38" t="s">
+      <c r="C142" s="32" t="s">
         <v>373</v>
       </c>
-      <c r="D142" s="38" t="s">
+      <c r="D142" s="32" t="s">
         <v>374</v>
       </c>
-      <c r="E142" s="38" t="s">
+      <c r="E142" s="32" t="s">
         <v>375</v>
       </c>
-      <c r="F142" s="38" t="s">
+      <c r="F142" s="32" t="s">
         <v>376</v>
       </c>
-      <c r="G142" s="38"/>
-      <c r="H142" s="38"/>
-      <c r="I142" s="38"/>
-      <c r="J142" s="38"/>
-      <c r="K142" s="38"/>
-      <c r="L142" s="38"/>
-      <c r="M142" s="39"/>
+      <c r="G142" s="32"/>
+      <c r="H142" s="32"/>
+      <c r="I142" s="32"/>
+      <c r="J142" s="32"/>
+      <c r="K142" s="32"/>
+      <c r="L142" s="32"/>
+      <c r="M142" s="33"/>
     </row>
     <row r="143" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B143" s="37" t="s">
+      <c r="B143" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="C143" s="38" t="s">
+      <c r="C143" s="32" t="s">
         <v>377</v>
       </c>
-      <c r="D143" s="38" t="s">
+      <c r="D143" s="32" t="s">
         <v>378</v>
       </c>
-      <c r="E143" s="38" t="s">
+      <c r="E143" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="F143" s="38" t="s">
+      <c r="F143" s="32" t="s">
         <v>380</v>
       </c>
-      <c r="G143" s="38"/>
-      <c r="H143" s="38"/>
-      <c r="I143" s="38"/>
-      <c r="J143" s="38"/>
-      <c r="K143" s="38"/>
-      <c r="L143" s="38"/>
-      <c r="M143" s="39"/>
+      <c r="G143" s="32"/>
+      <c r="H143" s="32"/>
+      <c r="I143" s="32"/>
+      <c r="J143" s="32"/>
+      <c r="K143" s="32"/>
+      <c r="L143" s="32"/>
+      <c r="M143" s="33"/>
     </row>
     <row r="144" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B144" s="37" t="s">
+      <c r="B144" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="C144" s="38" t="s">
+      <c r="C144" s="32" t="s">
         <v>381</v>
       </c>
-      <c r="D144" s="38" t="s">
+      <c r="D144" s="32" t="s">
         <v>382</v>
       </c>
-      <c r="E144" s="38" t="s">
+      <c r="E144" s="32" t="s">
         <v>383</v>
       </c>
-      <c r="F144" s="38" t="s">
+      <c r="F144" s="32" t="s">
         <v>384</v>
       </c>
-      <c r="G144" s="38"/>
-      <c r="H144" s="38"/>
-      <c r="I144" s="38"/>
-      <c r="J144" s="38"/>
-      <c r="K144" s="38"/>
-      <c r="L144" s="38"/>
-      <c r="M144" s="39"/>
+      <c r="G144" s="32"/>
+      <c r="H144" s="32"/>
+      <c r="I144" s="32"/>
+      <c r="J144" s="32"/>
+      <c r="K144" s="32"/>
+      <c r="L144" s="32"/>
+      <c r="M144" s="33"/>
     </row>
     <row r="145" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B145" s="37" t="s">
+      <c r="B145" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C145" s="38" t="s">
+      <c r="C145" s="32" t="s">
         <v>385</v>
       </c>
-      <c r="D145" s="38" t="s">
+      <c r="D145" s="32" t="s">
         <v>386</v>
       </c>
-      <c r="E145" s="38" t="s">
+      <c r="E145" s="32" t="s">
         <v>387</v>
       </c>
-      <c r="F145" s="38" t="s">
+      <c r="F145" s="32" t="s">
         <v>388</v>
       </c>
-      <c r="G145" s="38"/>
-      <c r="H145" s="38"/>
-      <c r="I145" s="38"/>
-      <c r="J145" s="38"/>
-      <c r="K145" s="38"/>
-      <c r="L145" s="38"/>
-      <c r="M145" s="39"/>
+      <c r="G145" s="32"/>
+      <c r="H145" s="32"/>
+      <c r="I145" s="32"/>
+      <c r="J145" s="32"/>
+      <c r="K145" s="32"/>
+      <c r="L145" s="32"/>
+      <c r="M145" s="33"/>
     </row>
     <row r="146" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B146" s="37" t="s">
+      <c r="B146" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="C146" s="38" t="s">
+      <c r="C146" s="32" t="s">
         <v>389</v>
       </c>
-      <c r="D146" s="38" t="s">
+      <c r="D146" s="32" t="s">
         <v>390</v>
       </c>
-      <c r="E146" s="38" t="s">
+      <c r="E146" s="32" t="s">
         <v>391</v>
       </c>
-      <c r="F146" s="38" t="s">
+      <c r="F146" s="32" t="s">
         <v>392</v>
       </c>
-      <c r="G146" s="38"/>
-      <c r="H146" s="38"/>
-      <c r="I146" s="38"/>
-      <c r="J146" s="38"/>
-      <c r="K146" s="38"/>
-      <c r="L146" s="38"/>
-      <c r="M146" s="39"/>
+      <c r="G146" s="32"/>
+      <c r="H146" s="32"/>
+      <c r="I146" s="32"/>
+      <c r="J146" s="32"/>
+      <c r="K146" s="32"/>
+      <c r="L146" s="32"/>
+      <c r="M146" s="33"/>
     </row>
     <row r="147" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B147" s="37" t="s">
+      <c r="B147" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="C147" s="38" t="s">
+      <c r="C147" s="32" t="s">
         <v>393</v>
       </c>
-      <c r="D147" s="38" t="s">
+      <c r="D147" s="32" t="s">
         <v>394</v>
       </c>
-      <c r="E147" s="38" t="s">
+      <c r="E147" s="32" t="s">
         <v>395</v>
       </c>
-      <c r="F147" s="38" t="s">
+      <c r="F147" s="32" t="s">
         <v>396</v>
       </c>
-      <c r="G147" s="38"/>
-      <c r="H147" s="38"/>
-      <c r="I147" s="38"/>
-      <c r="J147" s="38"/>
-      <c r="K147" s="38"/>
-      <c r="L147" s="38"/>
-      <c r="M147" s="39"/>
+      <c r="G147" s="32"/>
+      <c r="H147" s="32"/>
+      <c r="I147" s="32"/>
+      <c r="J147" s="32"/>
+      <c r="K147" s="32"/>
+      <c r="L147" s="32"/>
+      <c r="M147" s="33"/>
     </row>
     <row r="148" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B148" s="37" t="s">
+      <c r="B148" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="C148" s="38" t="s">
+      <c r="C148" s="32" t="s">
         <v>397</v>
       </c>
-      <c r="D148" s="38" t="s">
+      <c r="D148" s="32" t="s">
         <v>398</v>
       </c>
-      <c r="E148" s="38" t="s">
+      <c r="E148" s="32" t="s">
         <v>399</v>
       </c>
-      <c r="F148" s="38" t="s">
+      <c r="F148" s="32" t="s">
         <v>400</v>
       </c>
-      <c r="G148" s="38"/>
-      <c r="H148" s="38"/>
-      <c r="I148" s="38"/>
-      <c r="J148" s="38"/>
-      <c r="K148" s="38"/>
-      <c r="L148" s="38"/>
-      <c r="M148" s="39"/>
+      <c r="G148" s="32"/>
+      <c r="H148" s="32"/>
+      <c r="I148" s="32"/>
+      <c r="J148" s="32"/>
+      <c r="K148" s="32"/>
+      <c r="L148" s="32"/>
+      <c r="M148" s="33"/>
     </row>
     <row r="149" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B149" s="37" t="s">
+      <c r="B149" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="C149" s="38" t="s">
+      <c r="C149" s="32" t="s">
         <v>401</v>
       </c>
-      <c r="D149" s="38" t="s">
+      <c r="D149" s="32" t="s">
         <v>402</v>
       </c>
-      <c r="E149" s="38" t="s">
+      <c r="E149" s="32" t="s">
         <v>403</v>
       </c>
-      <c r="F149" s="38" t="s">
+      <c r="F149" s="32" t="s">
         <v>404</v>
       </c>
-      <c r="G149" s="38"/>
-      <c r="H149" s="38"/>
-      <c r="I149" s="38"/>
-      <c r="J149" s="38"/>
-      <c r="K149" s="38"/>
-      <c r="L149" s="38"/>
-      <c r="M149" s="39"/>
+      <c r="G149" s="32"/>
+      <c r="H149" s="32"/>
+      <c r="I149" s="32"/>
+      <c r="J149" s="32"/>
+      <c r="K149" s="32"/>
+      <c r="L149" s="32"/>
+      <c r="M149" s="33"/>
     </row>
     <row r="150" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B150" s="37" t="s">
+      <c r="B150" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C150" s="38" t="s">
+      <c r="C150" s="32" t="s">
         <v>405</v>
       </c>
-      <c r="D150" s="38" t="s">
+      <c r="D150" s="32" t="s">
         <v>406</v>
       </c>
-      <c r="E150" s="38" t="s">
+      <c r="E150" s="32" t="s">
         <v>407</v>
       </c>
-      <c r="F150" s="38" t="s">
+      <c r="F150" s="32" t="s">
         <v>408</v>
       </c>
-      <c r="G150" s="38"/>
-      <c r="H150" s="38"/>
-      <c r="I150" s="38"/>
-      <c r="J150" s="38"/>
-      <c r="K150" s="38"/>
-      <c r="L150" s="38"/>
-      <c r="M150" s="39"/>
+      <c r="G150" s="32"/>
+      <c r="H150" s="32"/>
+      <c r="I150" s="32"/>
+      <c r="J150" s="32"/>
+      <c r="K150" s="32"/>
+      <c r="L150" s="32"/>
+      <c r="M150" s="33"/>
     </row>
     <row r="151" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B151" s="37" t="s">
+      <c r="B151" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="C151" s="38" t="s">
+      <c r="C151" s="32" t="s">
         <v>409</v>
       </c>
-      <c r="D151" s="38" t="s">
+      <c r="D151" s="32" t="s">
         <v>410</v>
       </c>
-      <c r="E151" s="38" t="s">
+      <c r="E151" s="32" t="s">
         <v>411</v>
       </c>
-      <c r="F151" s="38" t="s">
+      <c r="F151" s="32" t="s">
         <v>412</v>
       </c>
-      <c r="G151" s="38"/>
-      <c r="H151" s="38"/>
-      <c r="I151" s="38"/>
-      <c r="J151" s="38"/>
-      <c r="K151" s="38"/>
-      <c r="L151" s="38"/>
-      <c r="M151" s="39"/>
+      <c r="G151" s="32"/>
+      <c r="H151" s="32"/>
+      <c r="I151" s="32"/>
+      <c r="J151" s="32"/>
+      <c r="K151" s="32"/>
+      <c r="L151" s="32"/>
+      <c r="M151" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>